<commit_message>
Add more links to docs, by @bycheng1
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="RTM" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RTM - Req from States + PreCert" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Selections" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -670,8 +670,8 @@
   </sheetPr>
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1232,7 +1232,7 @@
       <c r="E30" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G30" s="6"/>
@@ -1250,7 +1250,7 @@
       <c r="E31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G31" s="6"/>
@@ -1258,7 +1258,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="6" t="s">
         <v>45</v>
@@ -1268,7 +1268,7 @@
       <c r="E32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G32" s="6"/>
@@ -1286,7 +1286,7 @@
       <c r="E33" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G33" s="6"/>
@@ -1294,7 +1294,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="6" t="s">
         <v>47</v>
@@ -1304,7 +1304,7 @@
       <c r="E34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G34" s="6"/>
@@ -1312,7 +1312,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
       <c r="B35" s="6" t="s">
         <v>49</v>
@@ -1322,7 +1322,7 @@
       <c r="E35" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G35" s="6"/>
@@ -1340,7 +1340,7 @@
       <c r="E36" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G36" s="6"/>
@@ -1502,7 +1502,7 @@
       <c r="E45" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G45" s="6"/>
@@ -1520,7 +1520,7 @@
       <c r="E46" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G46" s="6"/>
@@ -1538,7 +1538,7 @@
       <c r="E47" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G47" s="6"/>
@@ -1556,7 +1556,7 @@
       <c r="E48" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F48" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G48" s="6"/>
@@ -1574,7 +1574,7 @@
       <c r="E49" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F49" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G49" s="6"/>
@@ -1592,7 +1592,7 @@
       <c r="E50" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G50" s="6"/>
@@ -2366,55 +2366,68 @@
     <hyperlink ref="F27" r:id="rId26" display="MISSOURI MEDICAID PROVIDER ENROLLMENT INFORMATION GUIDE.docx"/>
     <hyperlink ref="F28" r:id="rId27" display="MISSOURI MEDICAID PROVIDER ENROLLMENT INFORMATION GUIDE.docx"/>
     <hyperlink ref="F29" r:id="rId28" display="MISSOURI MEDICAID PROVIDER ENROLLMENT INFORMATION GUIDE.docx"/>
-    <hyperlink ref="F37" r:id="rId29" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F38" r:id="rId30" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F39" r:id="rId31" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F40" r:id="rId32" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F41" r:id="rId33" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F42" r:id="rId34" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F43" r:id="rId35" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F44" r:id="rId36" display="VTMedicaidProviderManual.pdf"/>
-    <hyperlink ref="F51" r:id="rId37" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F52" r:id="rId38" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F53" r:id="rId39" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F54" r:id="rId40" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F55" r:id="rId41" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F56" r:id="rId42" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F57" r:id="rId43" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F58" r:id="rId44" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F59" r:id="rId45" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F60" r:id="rId46" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F61" r:id="rId47" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F62" r:id="rId48" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F63" r:id="rId49" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F64" r:id="rId50" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F65" r:id="rId51" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F66" r:id="rId52" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F67" r:id="rId53" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F68" r:id="rId54" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F69" r:id="rId55" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F70" r:id="rId56" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F71" r:id="rId57" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F72" r:id="rId58" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F73" r:id="rId59" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F74" r:id="rId60" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F75" r:id="rId61" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F76" r:id="rId62" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F77" r:id="rId63" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F78" r:id="rId64" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F79" r:id="rId65" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F80" r:id="rId66" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F81" r:id="rId67" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F82" r:id="rId68" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F83" r:id="rId69" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F84" r:id="rId70" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F85" r:id="rId71" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F86" r:id="rId72" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F87" r:id="rId73" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F88" r:id="rId74" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F89" r:id="rId75" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F90" r:id="rId76" display="pre-certification-requirements.md"/>
-    <hyperlink ref="F91" r:id="rId77" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F30" r:id="rId29" display="PSM State Calls Requirements_functionality needs.xlsx"/>
+    <hyperlink ref="F31" r:id="rId30" display="PSM State Calls Requirements_functionality needs.xlsx"/>
+    <hyperlink ref="F32" r:id="rId31" display="PSM State Calls Requirements_functionality needs.xlsx"/>
+    <hyperlink ref="F33" r:id="rId32" display="PSM State Calls Requirements_functionality needs.xlsx"/>
+    <hyperlink ref="F34" r:id="rId33" display="PSM State Calls Requirements_functionality needs.xlsx"/>
+    <hyperlink ref="F35" r:id="rId34" display="PSM State Calls Requirements_functionality needs.xlsx"/>
+    <hyperlink ref="F36" r:id="rId35" display="PSM State Calls Requirements_functionality needs.xlsx"/>
+    <hyperlink ref="F37" r:id="rId36" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F38" r:id="rId37" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F39" r:id="rId38" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F40" r:id="rId39" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F41" r:id="rId40" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F42" r:id="rId41" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F43" r:id="rId42" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F44" r:id="rId43" display="VTMedicaidProviderManual.pdf"/>
+    <hyperlink ref="F45" r:id="rId44" display="GrnMtnCareEnrollInst.pdf"/>
+    <hyperlink ref="F46" r:id="rId45" display="GrnMtnCareEnrollInst.pdf"/>
+    <hyperlink ref="F47" r:id="rId46" display="GrnMtnCareEnrollInst.pdf"/>
+    <hyperlink ref="F48" r:id="rId47" display="GrnMtnCareEnrollInst.pdf"/>
+    <hyperlink ref="F49" r:id="rId48" display="GrnMtnCareEnrollInst.pdf"/>
+    <hyperlink ref="F50" r:id="rId49" display="GrnMtnCareEnrollInst.pdf"/>
+    <hyperlink ref="F51" r:id="rId50" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F52" r:id="rId51" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F53" r:id="rId52" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F54" r:id="rId53" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F55" r:id="rId54" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F56" r:id="rId55" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F57" r:id="rId56" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F58" r:id="rId57" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F59" r:id="rId58" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F60" r:id="rId59" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F61" r:id="rId60" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F62" r:id="rId61" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F63" r:id="rId62" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F64" r:id="rId63" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F65" r:id="rId64" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F66" r:id="rId65" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F67" r:id="rId66" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F68" r:id="rId67" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F69" r:id="rId68" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F70" r:id="rId69" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F71" r:id="rId70" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F72" r:id="rId71" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F73" r:id="rId72" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F74" r:id="rId73" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F75" r:id="rId74" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F76" r:id="rId75" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F77" r:id="rId76" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F78" r:id="rId77" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F79" r:id="rId78" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F80" r:id="rId79" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F81" r:id="rId80" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F82" r:id="rId81" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F83" r:id="rId82" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F84" r:id="rId83" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F85" r:id="rId84" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F86" r:id="rId85" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F87" r:id="rId86" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F88" r:id="rId87" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F89" r:id="rId88" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F90" r:id="rId89" display="pre-certification-requirements.md"/>
+    <hyperlink ref="F91" r:id="rId90" display="pre-certification-requirements.md"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added sequential IDs to each requirement
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mitre\CMS\CMCS\SGC\Phase 3 - MVP\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/dev/ots/psm/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7335" tabRatio="820"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12600" tabRatio="820"/>
   </bookViews>
   <sheets>
     <sheet name="FUNC Reqs" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FUNC Reqs'!$H$1:$H$92</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="247">
   <si>
     <t>MO</t>
   </si>
@@ -535,12 +541,264 @@
   </si>
   <si>
     <t>The PSM shall produce notices to applicants of pending status, approval, or rejection of their applications.</t>
+  </si>
+  <si>
+    <t>psm-1.1</t>
+  </si>
+  <si>
+    <t>psm-1.2</t>
+  </si>
+  <si>
+    <t>psm-1.3</t>
+  </si>
+  <si>
+    <t>psm-1.4</t>
+  </si>
+  <si>
+    <t>psm-1.5</t>
+  </si>
+  <si>
+    <t>psm-2.1</t>
+  </si>
+  <si>
+    <t>psm-2.2</t>
+  </si>
+  <si>
+    <t>psm-2.3</t>
+  </si>
+  <si>
+    <t>psm-2.4</t>
+  </si>
+  <si>
+    <t>psm-2.5</t>
+  </si>
+  <si>
+    <t>psm-2.6</t>
+  </si>
+  <si>
+    <t>psm-2.7</t>
+  </si>
+  <si>
+    <t>psm-2.8</t>
+  </si>
+  <si>
+    <t>psm-2.9</t>
+  </si>
+  <si>
+    <t>psm-2.10</t>
+  </si>
+  <si>
+    <t>psm-2.11</t>
+  </si>
+  <si>
+    <t>psm-2.12</t>
+  </si>
+  <si>
+    <t>psm-2.13</t>
+  </si>
+  <si>
+    <t>psm-2.14</t>
+  </si>
+  <si>
+    <t>psm-2.15</t>
+  </si>
+  <si>
+    <t>psm-2.16</t>
+  </si>
+  <si>
+    <t>psm-2.17</t>
+  </si>
+  <si>
+    <t>psm-2.18</t>
+  </si>
+  <si>
+    <t>psm-2.19</t>
+  </si>
+  <si>
+    <t>psm-3.1</t>
+  </si>
+  <si>
+    <t>psm-3.2</t>
+  </si>
+  <si>
+    <t>psm-3.3</t>
+  </si>
+  <si>
+    <t>psm-3.4</t>
+  </si>
+  <si>
+    <t>psm-3.5</t>
+  </si>
+  <si>
+    <t>psm-3.6</t>
+  </si>
+  <si>
+    <t>psm-3.7</t>
+  </si>
+  <si>
+    <t>psm-3.8</t>
+  </si>
+  <si>
+    <t>psm-3.9</t>
+  </si>
+  <si>
+    <t>psm-3.10</t>
+  </si>
+  <si>
+    <t>psm-3.11</t>
+  </si>
+  <si>
+    <t>psm-3.12</t>
+  </si>
+  <si>
+    <t>psm-3.13</t>
+  </si>
+  <si>
+    <t>psm-3.14</t>
+  </si>
+  <si>
+    <t>psm-3.15</t>
+  </si>
+  <si>
+    <t>psm-3.16</t>
+  </si>
+  <si>
+    <t>psm-3.17</t>
+  </si>
+  <si>
+    <t>psm-3.18</t>
+  </si>
+  <si>
+    <t>psm-3.19</t>
+  </si>
+  <si>
+    <t>psm-3.20</t>
+  </si>
+  <si>
+    <t>psm-3.21</t>
+  </si>
+  <si>
+    <t>psm-3.22</t>
+  </si>
+  <si>
+    <t>psm-3.23</t>
+  </si>
+  <si>
+    <t>psm-3.24</t>
+  </si>
+  <si>
+    <t>psm-4.1</t>
+  </si>
+  <si>
+    <t>psm-4.2</t>
+  </si>
+  <si>
+    <t>psm-4.3</t>
+  </si>
+  <si>
+    <t>psm-4.4</t>
+  </si>
+  <si>
+    <t>psm-4.5</t>
+  </si>
+  <si>
+    <t>psm-4.6</t>
+  </si>
+  <si>
+    <t>psm-4.7</t>
+  </si>
+  <si>
+    <t>psm-4.8</t>
+  </si>
+  <si>
+    <t>psm-4.9</t>
+  </si>
+  <si>
+    <t>psm-4.10</t>
+  </si>
+  <si>
+    <t>psm-4.11</t>
+  </si>
+  <si>
+    <t>psm-4.12</t>
+  </si>
+  <si>
+    <t>psm-4.13</t>
+  </si>
+  <si>
+    <t>psm-4.14</t>
+  </si>
+  <si>
+    <t>psm-4.15</t>
+  </si>
+  <si>
+    <t>psm-4.16</t>
+  </si>
+  <si>
+    <t>psm-5.1</t>
+  </si>
+  <si>
+    <t>psm-5.2</t>
+  </si>
+  <si>
+    <t>psm-5.3</t>
+  </si>
+  <si>
+    <t>psm-5.4</t>
+  </si>
+  <si>
+    <t>psm-6.1</t>
+  </si>
+  <si>
+    <t>psm-6.2</t>
+  </si>
+  <si>
+    <t>psm-7.1</t>
+  </si>
+  <si>
+    <t>psm-7.2</t>
+  </si>
+  <si>
+    <t>psm-7.3</t>
+  </si>
+  <si>
+    <t>psm-7.4</t>
+  </si>
+  <si>
+    <t>psm-7.5</t>
+  </si>
+  <si>
+    <t>psm-7.6</t>
+  </si>
+  <si>
+    <t>psm-7.7</t>
+  </si>
+  <si>
+    <t>psm-7.8</t>
+  </si>
+  <si>
+    <t>psm-7.9</t>
+  </si>
+  <si>
+    <t>psm-7.10</t>
+  </si>
+  <si>
+    <t>psm-7.11</t>
+  </si>
+  <si>
+    <t>psm-7.12</t>
+  </si>
+  <si>
+    <t>psm-7.13</t>
+  </si>
+  <si>
+    <t>psm-7.14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -709,42 +967,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -911,7 +1169,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1283,24 +1541,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K92"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="43" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.3984375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="32.86328125" style="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="32.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1335,7 +1593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="38" t="s">
         <v>96</v>
@@ -1350,8 +1608,10 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" ht="66" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>163</v>
+      </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>35</v>
@@ -1371,8 +1631,10 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="5"/>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
         <v>49</v>
@@ -1396,8 +1658,10 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>60</v>
@@ -1417,8 +1681,10 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="66" x14ac:dyDescent="0.45">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>166</v>
+      </c>
       <c r="B6" s="5"/>
       <c r="C6" s="36" t="s">
         <v>137</v>
@@ -1442,8 +1708,10 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="B7" s="5"/>
       <c r="C7" s="13" t="s">
         <v>144</v>
@@ -1463,7 +1731,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="38" t="s">
         <v>97</v>
@@ -1478,8 +1746,10 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="5"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>168</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="34" t="s">
         <v>103</v>
@@ -1502,8 +1772,10 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="B10" s="10"/>
       <c r="C10" s="33" t="s">
         <v>105</v>
@@ -1527,8 +1799,10 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6" t="s">
         <v>36</v>
@@ -1548,8 +1822,10 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>171</v>
+      </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="s">
         <v>45</v>
@@ -1573,8 +1849,10 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="s">
         <v>46</v>
@@ -1598,8 +1876,10 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="66" x14ac:dyDescent="0.45">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>173</v>
+      </c>
       <c r="B14" s="5"/>
       <c r="C14" s="6" t="s">
         <v>51</v>
@@ -1623,8 +1903,10 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="66" x14ac:dyDescent="0.45">
-      <c r="A15" s="5"/>
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
         <v>52</v>
@@ -1644,8 +1926,10 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="49.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>175</v>
+      </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="s">
         <v>55</v>
@@ -1665,8 +1949,10 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A17" s="5"/>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
         <v>56</v>
@@ -1690,8 +1976,10 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>177</v>
+      </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="s">
         <v>61</v>
@@ -1711,8 +1999,10 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="5"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>178</v>
+      </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
         <v>62</v>
@@ -1732,8 +2022,10 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="5"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>63</v>
@@ -1753,8 +2045,10 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="49.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="5"/>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>180</v>
+      </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
         <v>65</v>
@@ -1774,8 +2068,10 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="49.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="5"/>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
         <v>83</v>
@@ -1795,8 +2091,10 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A23" s="5"/>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="B23" s="37"/>
       <c r="C23" s="33" t="s">
         <v>91</v>
@@ -1820,8 +2118,10 @@
       <c r="J23" s="5"/>
       <c r="K23" s="35"/>
     </row>
-    <row r="24" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A24" s="5"/>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="B24" s="37"/>
       <c r="C24" s="33" t="s">
         <v>92</v>
@@ -1845,8 +2145,10 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A25" s="5"/>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="B25" s="5"/>
       <c r="C25" s="6" t="s">
         <v>94</v>
@@ -1866,8 +2168,10 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A26" s="5"/>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="B26" s="11"/>
       <c r="C26" s="13" t="s">
         <v>143</v>
@@ -1887,8 +2191,10 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="49.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="5"/>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>186</v>
+      </c>
       <c r="B27" s="11"/>
       <c r="C27" s="6" t="s">
         <v>109</v>
@@ -1907,7 +2213,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="38" t="s">
         <v>98</v>
@@ -1922,8 +2228,10 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="5"/>
+    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>187</v>
+      </c>
       <c r="B29" s="5"/>
       <c r="C29" s="13" t="s">
         <v>106</v>
@@ -1943,8 +2251,10 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A30" s="5"/>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="B30" s="5"/>
       <c r="C30" s="6" t="s">
         <v>30</v>
@@ -1963,8 +2273,10 @@
       <c r="I30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A31" s="5"/>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="B31" s="5"/>
       <c r="C31" s="6" t="s">
         <v>32</v>
@@ -1984,8 +2296,10 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A32" s="5"/>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B32" s="5"/>
       <c r="C32" s="6" t="s">
         <v>33</v>
@@ -2005,8 +2319,10 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A33" s="5"/>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="B33" s="5"/>
       <c r="C33" s="6" t="s">
         <v>53</v>
@@ -2026,8 +2342,10 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="5"/>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="B34" s="5"/>
       <c r="C34" s="6" t="s">
         <v>54</v>
@@ -2047,8 +2365,10 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" ht="115.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="5"/>
+    <row r="35" spans="1:11" ht="90" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>193</v>
+      </c>
       <c r="B35" s="5"/>
       <c r="C35" s="6" t="s">
         <v>57</v>
@@ -2068,8 +2388,10 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="5"/>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>194</v>
+      </c>
       <c r="B36" s="5"/>
       <c r="C36" s="6" t="s">
         <v>66</v>
@@ -2089,8 +2411,10 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="5"/>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>195</v>
+      </c>
       <c r="B37" s="37"/>
       <c r="C37" s="33" t="s">
         <v>70</v>
@@ -2114,8 +2438,10 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A38" s="5"/>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>196</v>
+      </c>
       <c r="B38" s="37"/>
       <c r="C38" s="33" t="s">
         <v>71</v>
@@ -2139,8 +2465,10 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A39" s="5"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>197</v>
+      </c>
       <c r="B39" s="5"/>
       <c r="C39" s="6" t="s">
         <v>72</v>
@@ -2160,8 +2488,10 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A40" s="5"/>
+    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="B40" s="5"/>
       <c r="C40" s="6" t="s">
         <v>73</v>
@@ -2185,8 +2515,10 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11" ht="115.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="5"/>
+    <row r="41" spans="1:11" ht="90" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>199</v>
+      </c>
       <c r="B41" s="5"/>
       <c r="C41" s="6" t="s">
         <v>74</v>
@@ -2206,8 +2538,10 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A42" s="5"/>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="B42" s="5"/>
       <c r="C42" s="6" t="s">
         <v>75</v>
@@ -2227,8 +2561,10 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
-    <row r="43" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A43" s="5"/>
+    <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>201</v>
+      </c>
       <c r="B43" s="5"/>
       <c r="C43" s="6" t="s">
         <v>76</v>
@@ -2248,8 +2584,10 @@
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
     </row>
-    <row r="44" spans="1:11" ht="198" x14ac:dyDescent="0.45">
-      <c r="A44" s="5"/>
+    <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="B44" s="5"/>
       <c r="C44" s="6" t="s">
         <v>77</v>
@@ -2269,8 +2607,10 @@
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
     </row>
-    <row r="45" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A45" s="5"/>
+    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="B45" s="5"/>
       <c r="C45" s="6" t="s">
         <v>78</v>
@@ -2290,8 +2630,10 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A46" s="5"/>
+    <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="B46" s="5"/>
       <c r="C46" s="6" t="s">
         <v>79</v>
@@ -2311,8 +2653,10 @@
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
     </row>
-    <row r="47" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A47" s="5"/>
+    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="B47" s="5"/>
       <c r="C47" s="33" t="s">
         <v>84</v>
@@ -2332,8 +2676,10 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A48" s="5"/>
+    <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="B48" s="5"/>
       <c r="C48" s="6" t="s">
         <v>85</v>
@@ -2353,8 +2699,10 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" spans="1:11" ht="49.5" x14ac:dyDescent="0.45">
-      <c r="A49" s="5"/>
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="B49" s="5"/>
       <c r="C49" s="6" t="s">
         <v>89</v>
@@ -2374,8 +2722,10 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A50" s="5"/>
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="B50" s="5"/>
       <c r="C50" s="6" t="s">
         <v>93</v>
@@ -2395,8 +2745,10 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" spans="1:11" ht="66" x14ac:dyDescent="0.45">
-      <c r="A51" s="5"/>
+    <row r="51" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>209</v>
+      </c>
       <c r="B51" s="5"/>
       <c r="C51" s="6" t="s">
         <v>110</v>
@@ -2416,8 +2768,10 @@
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
     </row>
-    <row r="52" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A52" s="5"/>
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="B52" s="5"/>
       <c r="C52" s="6" t="s">
         <v>139</v>
@@ -2437,7 +2791,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
     </row>
-    <row r="53" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8"/>
       <c r="B53" s="38" t="s">
         <v>99</v>
@@ -2452,8 +2806,10 @@
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="1:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="5"/>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="B54" s="5"/>
       <c r="C54" s="6" t="s">
         <v>31</v>
@@ -2473,8 +2829,10 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
     </row>
-    <row r="55" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A55" s="5"/>
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="B55" s="5"/>
       <c r="C55" s="6" t="s">
         <v>34</v>
@@ -2494,8 +2852,10 @@
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
     </row>
-    <row r="56" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A56" s="5"/>
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>213</v>
+      </c>
       <c r="B56" s="5"/>
       <c r="C56" s="6" t="s">
         <v>39</v>
@@ -2515,8 +2875,10 @@
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
     </row>
-    <row r="57" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A57" s="5"/>
+    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="B57" s="5"/>
       <c r="C57" s="6" t="s">
         <v>40</v>
@@ -2536,8 +2898,10 @@
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
     </row>
-    <row r="58" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A58" s="5"/>
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="B58" s="5"/>
       <c r="C58" s="6" t="s">
         <v>41</v>
@@ -2561,8 +2925,10 @@
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
     </row>
-    <row r="59" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A59" s="5"/>
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="B59" s="5"/>
       <c r="C59" s="6" t="s">
         <v>42</v>
@@ -2586,8 +2952,10 @@
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
     </row>
-    <row r="60" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A60" s="5"/>
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="B60" s="5"/>
       <c r="C60" s="6" t="s">
         <v>43</v>
@@ -2611,8 +2979,10 @@
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
     </row>
-    <row r="61" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A61" s="5"/>
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="B61" s="5"/>
       <c r="C61" s="6" t="s">
         <v>44</v>
@@ -2636,8 +3006,10 @@
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
     </row>
-    <row r="62" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A62" s="5"/>
+    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>219</v>
+      </c>
       <c r="B62" s="5"/>
       <c r="C62" s="6" t="s">
         <v>47</v>
@@ -2661,8 +3033,10 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
     </row>
-    <row r="63" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A63" s="5"/>
+    <row r="63" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="B63" s="5"/>
       <c r="C63" s="6" t="s">
         <v>48</v>
@@ -2686,8 +3060,10 @@
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
     </row>
-    <row r="64" spans="1:11" ht="49.5" x14ac:dyDescent="0.45">
-      <c r="A64" s="5"/>
+    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="B64" s="5"/>
       <c r="C64" s="6" t="s">
         <v>59</v>
@@ -2707,8 +3083,10 @@
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
     </row>
-    <row r="65" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A65" s="5"/>
+    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="B65" s="5"/>
       <c r="C65" s="6" t="s">
         <v>64</v>
@@ -2732,8 +3110,10 @@
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
     </row>
-    <row r="66" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A66" s="5"/>
+    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="B66" s="5"/>
       <c r="C66" s="6" t="s">
         <v>81</v>
@@ -2753,8 +3133,10 @@
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
     </row>
-    <row r="67" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A67" s="5"/>
+    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="B67" s="5"/>
       <c r="C67" s="6" t="s">
         <v>86</v>
@@ -2774,8 +3156,10 @@
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
     </row>
-    <row r="68" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A68" s="5"/>
+    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="B68" s="5"/>
       <c r="C68" s="6" t="s">
         <v>90</v>
@@ -2795,8 +3179,10 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
     </row>
-    <row r="69" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A69" s="5"/>
+    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="B69" s="5"/>
       <c r="C69" s="6" t="s">
         <v>162</v>
@@ -2816,7 +3202,7 @@
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
     </row>
-    <row r="70" spans="1:11" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="38" t="s">
         <v>100</v>
@@ -2831,8 +3217,10 @@
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
     </row>
-    <row r="71" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A71" s="5"/>
+    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="B71" s="5"/>
       <c r="C71" s="6" t="s">
         <v>37</v>
@@ -2851,8 +3239,10 @@
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
     </row>
-    <row r="72" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A72" s="5"/>
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>228</v>
+      </c>
       <c r="B72" s="5"/>
       <c r="C72" s="6" t="s">
         <v>38</v>
@@ -2872,8 +3262,10 @@
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
     </row>
-    <row r="73" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A73" s="5"/>
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="B73" s="5"/>
       <c r="C73" s="6" t="s">
         <v>82</v>
@@ -2893,8 +3285,10 @@
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
     </row>
-    <row r="74" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A74" s="5"/>
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="B74" s="5"/>
       <c r="C74" s="6" t="s">
         <v>87</v>
@@ -2914,7 +3308,7 @@
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
     </row>
-    <row r="75" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8"/>
       <c r="B75" s="38" t="s">
         <v>101</v>
@@ -2929,8 +3323,10 @@
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
     </row>
-    <row r="76" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A76" s="5"/>
+    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="B76" s="5"/>
       <c r="C76" s="6" t="s">
         <v>50</v>
@@ -2950,8 +3346,10 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
     </row>
-    <row r="77" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A77" s="5"/>
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>232</v>
+      </c>
       <c r="B77" s="5"/>
       <c r="C77" s="6" t="s">
         <v>58</v>
@@ -2971,7 +3369,7 @@
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
     </row>
-    <row r="78" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="B78" s="38" t="s">
         <v>102</v>
@@ -2986,8 +3384,10 @@
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
     </row>
-    <row r="79" spans="1:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A79" s="5"/>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>233</v>
+      </c>
       <c r="B79" s="5"/>
       <c r="C79" s="6" t="s">
         <v>67</v>
@@ -3007,8 +3407,10 @@
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
     </row>
-    <row r="80" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A80" s="5"/>
+    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B80" s="5"/>
       <c r="C80" s="6" t="s">
         <v>68</v>
@@ -3028,8 +3430,10 @@
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
     </row>
-    <row r="81" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A81" s="5"/>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>235</v>
+      </c>
       <c r="B81" s="5"/>
       <c r="C81" s="6" t="s">
         <v>69</v>
@@ -3053,8 +3457,10 @@
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
     </row>
-    <row r="82" spans="1:11" ht="66" x14ac:dyDescent="0.45">
-      <c r="A82" s="5"/>
+    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>236</v>
+      </c>
       <c r="B82" s="5"/>
       <c r="C82" s="32" t="s">
         <v>138</v>
@@ -3074,8 +3480,10 @@
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
     </row>
-    <row r="83" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A83" s="5"/>
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
+        <v>237</v>
+      </c>
       <c r="B83" s="5"/>
       <c r="C83" s="6" t="s">
         <v>88</v>
@@ -3095,8 +3503,10 @@
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
     </row>
-    <row r="84" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A84" s="5"/>
+    <row r="84" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>238</v>
+      </c>
       <c r="B84" s="5"/>
       <c r="C84" s="6" t="s">
         <v>111</v>
@@ -3120,8 +3530,10 @@
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
     </row>
-    <row r="85" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A85" s="5"/>
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>239</v>
+      </c>
       <c r="B85" s="5"/>
       <c r="C85" s="6" t="s">
         <v>140</v>
@@ -3141,8 +3553,10 @@
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
     </row>
-    <row r="86" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A86" s="5"/>
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
+        <v>240</v>
+      </c>
       <c r="B86" s="5"/>
       <c r="C86" s="6" t="s">
         <v>112</v>
@@ -3162,8 +3576,10 @@
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
     </row>
-    <row r="87" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A87" s="5"/>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>241</v>
+      </c>
       <c r="B87" s="5"/>
       <c r="C87" s="6" t="s">
         <v>113</v>
@@ -3183,8 +3599,10 @@
       <c r="J87" s="5"/>
       <c r="K87" s="5"/>
     </row>
-    <row r="88" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A88" s="5"/>
+    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>242</v>
+      </c>
       <c r="B88" s="5"/>
       <c r="C88" s="6" t="s">
         <v>114</v>
@@ -3204,8 +3622,10 @@
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
     </row>
-    <row r="89" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A89" s="5"/>
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>243</v>
+      </c>
       <c r="B89" s="5"/>
       <c r="C89" s="6" t="s">
         <v>80</v>
@@ -3225,8 +3645,10 @@
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
     </row>
-    <row r="90" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A90" s="5"/>
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>244</v>
+      </c>
       <c r="B90" s="5"/>
       <c r="C90" s="6" t="s">
         <v>115</v>
@@ -3246,8 +3668,10 @@
       <c r="J90" s="5"/>
       <c r="K90" s="5"/>
     </row>
-    <row r="91" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A91" s="5"/>
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>245</v>
+      </c>
       <c r="B91" s="5"/>
       <c r="C91" s="6" t="s">
         <v>116</v>
@@ -3267,8 +3691,10 @@
       <c r="J91" s="5"/>
       <c r="K91" s="5"/>
     </row>
-    <row r="92" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A92" s="5"/>
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="B92" s="5"/>
       <c r="C92" s="6" t="s">
         <v>117</v>
@@ -3365,21 +3791,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="15"/>
-    <col min="2" max="2" width="71.73046875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="16" t="s">
         <v>118</v>
       </c>
@@ -3391,7 +3817,7 @@
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
     </row>
-    <row r="2" spans="2:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>120</v>
       </c>
@@ -3406,7 +3832,7 @@
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
     </row>
-    <row r="3" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
         <v>136</v>
       </c>
@@ -3420,7 +3846,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
         <v>135</v>
       </c>
@@ -3430,7 +3856,7 @@
       </c>
       <c r="E4" s="26"/>
     </row>
-    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="30" t="s">
         <v>134</v>
       </c>
@@ -3440,7 +3866,7 @@
       </c>
       <c r="E5" s="26"/>
     </row>
-    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="31" t="s">
         <v>133</v>
       </c>
@@ -3450,7 +3876,7 @@
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="30" t="s">
         <v>132</v>
       </c>
@@ -3460,7 +3886,7 @@
       </c>
       <c r="E7" s="26"/>
     </row>
-    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="30" t="s">
         <v>131</v>
       </c>
@@ -3470,7 +3896,7 @@
       </c>
       <c r="E8" s="26"/>
     </row>
-    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="30" t="s">
         <v>130</v>
       </c>
@@ -3480,7 +3906,7 @@
       </c>
       <c r="E9" s="26"/>
     </row>
-    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="30" t="s">
         <v>129</v>
       </c>
@@ -3490,7 +3916,7 @@
       </c>
       <c r="E10" s="26"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C11" s="22" t="s">
         <v>126</v>
       </c>
@@ -3499,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C12" s="15" t="s">
         <v>127</v>
       </c>
@@ -3508,7 +3934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C13" s="15" t="s">
         <v>128</v>
       </c>
@@ -3542,9 +3968,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3555,7 +3981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3566,7 +3992,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3577,7 +4003,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3588,7 +4014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3596,12 +4022,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>28</v>
       </c>
@@ -3612,33 +4038,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Training_x0020_Document xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">false</Training_x0020_Document>
-    <Status xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">In Progress</Status>
-    <Path_All xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b" xsi:nil="true"/>
-    <State xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">N/A</State>
-    <_Contributor xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Project_x002f_Task xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">Provider Screening</Project_x002f_Task>
-    <Comments_from_Title xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b" xsi:nil="true"/>
-    <Document_x0020_Owner xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">Cheng, Bill Y.</Document_x0020_Owner>
-    <MITRE_x0020_Sensitivity xmlns="http://schemas.microsoft.com/sharepoint/v3">Internal MITRE Information</MITRE_x0020_Sensitivity>
-    <Release_x0020_Statement xmlns="http://schemas.microsoft.com/sharepoint/v3">For Internal MITRE Use</Release_x0020_Statement>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Working Document" ma:contentTypeID="0x010100823A99C636F7423283FB0D200866C61300AE1A2994EE84A84F9E74D345EED6B3D10088ECA138718353438D4A052900881425" ma:contentTypeVersion="16" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2a4c09df1e3a62c3b12fd7b7bb235f29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4d3e69fe-1b8b-4540-be82-e253ea88466b" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc421a2e084d263ad97b084ca96adad2" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3934,42 +4342,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Training_x0020_Document xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">false</Training_x0020_Document>
+    <Status xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">In Progress</Status>
+    <Path_All xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b" xsi:nil="true"/>
+    <State xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">N/A</State>
+    <_Contributor xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Project_x002f_Task xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">Provider Screening</Project_x002f_Task>
+    <Comments_from_Title xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b" xsi:nil="true"/>
+    <Document_x0020_Owner xmlns="4d3e69fe-1b8b-4540-be82-e253ea88466b">Cheng, Bill Y.</Document_x0020_Owner>
+    <MITRE_x0020_Sensitivity xmlns="http://schemas.microsoft.com/sharepoint/v3">Internal MITRE Information</MITRE_x0020_Sensitivity>
+    <Release_x0020_Statement xmlns="http://schemas.microsoft.com/sharepoint/v3">For Internal MITRE Use</Release_x0020_Statement>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B3-F88D-47E7-B797-DF0C796DC9A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5057FD5-666C-43F9-B052-DCBEC34E095F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4d3e69fe-1b8b-4540-be82-e253ea88466b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56C8154B-3453-4080-801A-FE2EC194234B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3879E760-9447-4C31-8A25-266CCF95C142}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3989,10 +4397,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56C8154B-3453-4080-801A-FE2EC194234B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5057FD5-666C-43F9-B052-DCBEC34E095F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B3-F88D-47E7-B797-DF0C796DC9A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4d3e69fe-1b8b-4540-be82-e253ea88466b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Freeze the first row of the RTM spreadsheet
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -2520,7 +2520,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2573,10 +2573,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2595,10 +2591,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2629,16 +2621,8 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -2655,10 +2639,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2781,8 +2761,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2882,9 +2862,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1913760</xdr:colOff>
+      <xdr:colOff>1913400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2894,7 +2874,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="634680" y="0"/>
-          <a:ext cx="1913760" cy="676080"/>
+          <a:ext cx="1913400" cy="675720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2949,18 +2929,20 @@
   </sheetPr>
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="73.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="32.87"/>
@@ -3098,7 +3080,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="7" t="n">
@@ -3125,7 +3107,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="7"/>
@@ -3133,10 +3115,10 @@
       <c r="F7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I7" s="10"/>
@@ -3171,7 +3153,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="6" t="s">
         <v>41</v>
       </c>
@@ -3190,19 +3172,19 @@
         <v>42</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="14" t="n">
+      <c r="D10" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>44</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -3212,11 +3194,11 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="7" t="n">
@@ -3225,10 +3207,10 @@
       <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>44</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -3262,7 +3244,7 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="10"/>
@@ -3316,7 +3298,7 @@
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="99.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B15" s="10"/>
@@ -3368,7 +3350,7 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B17" s="10"/>
@@ -3422,7 +3404,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B19" s="10"/>
@@ -3468,7 +3450,7 @@
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="10"/>
@@ -3514,7 +3496,7 @@
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="71.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="15" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="10"/>
@@ -3542,8 +3524,8 @@
       <c r="A24" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D24" s="7" t="n">
@@ -3568,11 +3550,11 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="14" t="s">
+      <c r="B25" s="10"/>
+      <c r="C25" s="13" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="7" t="n">
@@ -3618,11 +3600,11 @@
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="14" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="13" t="s">
         <v>93</v>
       </c>
       <c r="D27" s="7"/>
@@ -3630,10 +3612,10 @@
       <c r="F27" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>94</v>
       </c>
       <c r="I27" s="10"/>
@@ -3644,7 +3626,7 @@
       <c r="A28" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="20"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="7" t="s">
         <v>96</v>
       </c>
@@ -3653,10 +3635,10 @@
       <c r="F28" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="13" t="s">
         <v>94</v>
       </c>
       <c r="J28" s="10"/>
@@ -3690,7 +3672,7 @@
       <c r="K29" s="10"/>
     </row>
     <row r="30" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="6" t="s">
         <v>100</v>
       </c>
@@ -3709,7 +3691,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="10"/>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>102</v>
       </c>
       <c r="D31" s="7"/>
@@ -3720,7 +3702,7 @@
       <c r="G31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="8"/>
@@ -3755,7 +3737,7 @@
         <v>105</v>
       </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D33" s="7"/>
@@ -3766,7 +3748,7 @@
       <c r="G33" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I33" s="10"/>
@@ -3907,10 +3889,10 @@
       <c r="F39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="15" t="s">
+      <c r="G39" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I39" s="10"/>
@@ -4055,7 +4037,7 @@
       <c r="F45" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G45" s="14" t="s">
         <v>36</v>
       </c>
       <c r="H45" s="7" t="s">
@@ -4078,10 +4060,10 @@
       <c r="F46" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G46" s="15" t="s">
+      <c r="G46" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H46" s="13" t="s">
+      <c r="H46" s="7" t="s">
         <v>94</v>
       </c>
       <c r="I46" s="10"/>
@@ -4101,10 +4083,10 @@
       <c r="F47" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H47" s="13" t="s">
+      <c r="H47" s="7" t="s">
         <v>94</v>
       </c>
       <c r="I47" s="10"/>
@@ -4124,10 +4106,10 @@
       <c r="F48" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H48" s="13" t="s">
+      <c r="H48" s="7" t="s">
         <v>94</v>
       </c>
       <c r="I48" s="10"/>
@@ -4147,10 +4129,10 @@
       <c r="F49" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H49" s="13" t="s">
+      <c r="H49" s="7" t="s">
         <v>94</v>
       </c>
       <c r="I49" s="10"/>
@@ -4170,7 +4152,7 @@
       <c r="F50" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G50" s="14" t="s">
         <v>36</v>
       </c>
       <c r="H50" s="7" t="s">
@@ -4193,10 +4175,10 @@
       <c r="F51" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G51" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H51" s="13" t="s">
+      <c r="H51" s="7" t="s">
         <v>94</v>
       </c>
       <c r="I51" s="10"/>
@@ -4216,10 +4198,10 @@
       <c r="F52" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="G52" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H52" s="13" t="s">
+      <c r="H52" s="7" t="s">
         <v>94</v>
       </c>
       <c r="I52" s="10"/>
@@ -4239,7 +4221,7 @@
       <c r="F53" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="14" t="s">
         <v>36</v>
       </c>
       <c r="H53" s="7" t="s">
@@ -4277,7 +4259,7 @@
       <c r="K54" s="10"/>
     </row>
     <row r="55" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="16"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="6" t="s">
         <v>159</v>
       </c>
@@ -4342,7 +4324,7 @@
         <v>164</v>
       </c>
       <c r="B58" s="10"/>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="13" t="s">
         <v>165</v>
       </c>
       <c r="D58" s="7"/>
@@ -4358,7 +4340,7 @@
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="21"/>
+      <c r="K58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
@@ -4411,7 +4393,7 @@
       <c r="K60" s="10"/>
     </row>
     <row r="61" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="6" t="s">
         <v>172</v>
       </c>
@@ -4454,8 +4436,8 @@
       <c r="A63" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="B63" s="19"/>
-      <c r="C63" s="14" t="s">
+      <c r="B63" s="10"/>
+      <c r="C63" s="13" t="s">
         <v>177</v>
       </c>
       <c r="D63" s="7" t="n">
@@ -4483,8 +4465,8 @@
       <c r="A64" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B64" s="19"/>
-      <c r="C64" s="14" t="s">
+      <c r="B64" s="10"/>
+      <c r="C64" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D64" s="7" t="n">
@@ -4527,7 +4509,7 @@
       </c>
       <c r="I65" s="10"/>
       <c r="J65" s="10"/>
-      <c r="K65" s="21"/>
+      <c r="K65" s="19"/>
     </row>
     <row r="66" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
@@ -4545,7 +4527,7 @@
       <c r="G66" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H66" s="13" t="s">
+      <c r="H66" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I66" s="10"/>
@@ -4557,7 +4539,7 @@
         <v>186</v>
       </c>
       <c r="B67" s="10"/>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="13" t="s">
         <v>187</v>
       </c>
       <c r="D67" s="7"/>
@@ -4573,14 +4555,14 @@
       </c>
       <c r="I67" s="10"/>
       <c r="J67" s="10"/>
-      <c r="K67" s="21"/>
+      <c r="K67" s="19"/>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
         <v>188</v>
       </c>
       <c r="B68" s="10"/>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="13" t="s">
         <v>189</v>
       </c>
       <c r="D68" s="7"/>
@@ -4594,14 +4576,14 @@
       </c>
       <c r="I68" s="10"/>
       <c r="J68" s="10"/>
-      <c r="K68" s="21"/>
+      <c r="K68" s="19"/>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
         <v>190</v>
       </c>
       <c r="B69" s="10"/>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="13" t="s">
         <v>191</v>
       </c>
       <c r="D69" s="7"/>
@@ -4610,7 +4592,7 @@
         <v>70</v>
       </c>
       <c r="G69" s="11"/>
-      <c r="H69" s="13" t="s">
+      <c r="H69" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I69" s="10"/>
@@ -4618,7 +4600,7 @@
       <c r="K69" s="10"/>
     </row>
     <row r="70" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="16"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="6" t="s">
         <v>192</v>
       </c>
@@ -4714,10 +4696,10 @@
       <c r="F74" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="G74" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H74" s="13" t="s">
+      <c r="H74" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I74" s="10"/>
@@ -4769,7 +4751,7 @@
         <v>49</v>
       </c>
       <c r="I76" s="10"/>
-      <c r="K76" s="21"/>
+      <c r="K76" s="19"/>
     </row>
     <row r="77" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
@@ -4799,7 +4781,7 @@
         <v>210</v>
       </c>
       <c r="B78" s="10"/>
-      <c r="C78" s="22" t="s">
+      <c r="C78" s="20" t="s">
         <v>211</v>
       </c>
       <c r="D78" s="7"/>
@@ -4812,10 +4794,10 @@
         <v>49</v>
       </c>
       <c r="I78" s="10"/>
-      <c r="K78" s="23"/>
+      <c r="K78" s="21"/>
     </row>
     <row r="79" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="16"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="6" t="s">
         <v>212</v>
       </c>
@@ -5004,7 +4986,7 @@
       </c>
       <c r="I86" s="10"/>
       <c r="J86" s="10"/>
-      <c r="K86" s="21"/>
+      <c r="K86" s="19"/>
     </row>
     <row r="87" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
@@ -5115,7 +5097,7 @@
         <v>235</v>
       </c>
       <c r="B91" s="10"/>
-      <c r="C91" s="14" t="s">
+      <c r="C91" s="13" t="s">
         <v>236</v>
       </c>
       <c r="D91" s="7"/>
@@ -5132,7 +5114,7 @@
       <c r="K91" s="10"/>
     </row>
     <row r="92" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="16"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="6" t="s">
         <v>237</v>
       </c>
@@ -5167,7 +5149,7 @@
       </c>
       <c r="I93" s="10"/>
       <c r="J93" s="10"/>
-      <c r="K93" s="21"/>
+      <c r="K93" s="19"/>
     </row>
     <row r="94" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
@@ -5243,7 +5225,7 @@
         <v>250</v>
       </c>
       <c r="B97" s="10"/>
-      <c r="C97" s="14" t="s">
+      <c r="C97" s="13" t="s">
         <v>251</v>
       </c>
       <c r="D97" s="7"/>
@@ -5260,7 +5242,7 @@
       <c r="K97" s="10"/>
     </row>
     <row r="98" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="16"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="6" t="s">
         <v>252</v>
       </c>
@@ -5393,7 +5375,7 @@
       <c r="K103" s="10"/>
     </row>
     <row r="104" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="16"/>
+      <c r="A104" s="15"/>
       <c r="B104" s="6" t="s">
         <v>266</v>
       </c>
@@ -5415,8 +5397,8 @@
       <c r="C105" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D105" s="24"/>
-      <c r="E105" s="24"/>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
       <c r="F105" s="7" t="s">
         <v>14</v>
       </c>
@@ -5445,16 +5427,16 @@
     <mergeCell ref="B104:C104"/>
   </mergeCells>
   <dataValidations count="5">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E8 E10:E29 E31:E47 E54 E56:E60 E62:E69 E71:E78 E80:E91 E93:E95 E97 E99:E103 E105" type="list">
+      <formula1>Selections!$B$4:$B$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5 H7 H12 H16:H17 H19:H23 H26:H28 H40:H41 H43:H44 H46:H53 H71 H75 H80:H82 H89 H91 H93:H97 H99:H102 H105" type="list">
       <formula1>$C$5:$C$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D8 D10:D29 D31:D47 D54 D56:D60 D62:D69 D71:D78 D80:D91 D93:D95 D97 D99:D103 D105" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E8 E10:E29 E31:E47 E54 E56:E60 E62:E69 E71:E78 E80:E91 E93:E95 E97 E99:E103 E105" type="list">
-      <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H31:H33 H35:H39 H56:H59 H62 H65:H69 H72:H74 H76:H78" type="list">
@@ -5524,386 +5506,386 @@
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="32.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="D3" s="29" t="n">
+      <c r="D3" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-    </row>
-    <row r="4" s="27" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="32" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="33" t="s">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="29" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="32" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30" t="s">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-    </row>
-    <row r="7" s="34" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="D7" s="29" t="n">
+      <c r="D7" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="28" t="s">
         <v>283</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30" t="s">
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="8" s="34" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
+    <row r="8" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="32" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30" t="s">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-    </row>
-    <row r="9" s="34" customFormat="true" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="32" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="35" t="s">
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="30" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="10" s="27" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23"/>
+      <c r="B10" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="32" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="28" t="s">
         <v>295</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="32" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="28" t="s">
         <v>298</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="33" t="s">
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="29" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="13" s="27" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25"/>
-      <c r="B13" s="28" t="s">
+    <row r="13" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23"/>
+      <c r="B13" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="28" t="s">
         <v>303</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-    </row>
-    <row r="16" s="34" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="27" t="s">
         <v>308</v>
       </c>
-      <c r="D16" s="29" t="n">
+      <c r="D16" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="30" t="s">
+      <c r="G16" s="24"/>
+      <c r="H16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="36"/>
-    </row>
-    <row r="17" s="34" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="D17" s="29" t="n">
+      <c r="D17" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="30" t="s">
+      <c r="G17" s="24"/>
+      <c r="H17" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="36"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="H1:H17"/>
@@ -5951,317 +5933,317 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="19.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="73.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="6.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="14.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="34" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="34" width="32.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="32.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33" t="s">
         <v>315</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-    </row>
-    <row r="4" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="32" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="39" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="35" t="s">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="30" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="6" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28" t="s">
+    <row r="6" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23"/>
+      <c r="B6" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="32" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30" t="s">
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="8" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28" t="s">
+    <row r="8" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23"/>
+      <c r="B8" s="25" t="s">
         <v>326</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-    </row>
-    <row r="9" s="27" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="31" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="27" t="s">
         <v>327</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="40" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="25" t="s">
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="23" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="10" s="27" customFormat="true" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
+    <row r="10" s="4" customFormat="true" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="D10" s="29" t="n">
+      <c r="D10" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="30" t="s">
+      <c r="G10" s="24"/>
+      <c r="H10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="36" t="s">
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="31" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="11" s="27" customFormat="true" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+    <row r="11" s="4" customFormat="true" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="27" t="s">
         <v>334</v>
       </c>
-      <c r="D11" s="29" t="n">
+      <c r="D11" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="30" t="s">
+      <c r="G11" s="24"/>
+      <c r="H11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="36" t="s">
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="31" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="12" s="27" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+    <row r="12" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="32" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="28" t="s">
         <v>338</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="24"/>
+      <c r="H12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-    </row>
-    <row r="13" s="27" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" s="4" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="D13" s="29" t="n">
+      <c r="D13" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="30" t="s">
+      <c r="G13" s="24"/>
+      <c r="H13" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-    </row>
-    <row r="14" s="27" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" s="4" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="27" t="s">
         <v>343</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="28" t="s">
         <v>344</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="30" t="s">
+      <c r="G14" s="24"/>
+      <c r="H14" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
     </row>
   </sheetData>
   <autoFilter ref="H1:H14">
@@ -6315,497 +6297,497 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="19.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="73.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="6.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="14.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="34" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="34" width="32.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="32.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33" t="s">
         <v>348</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="32" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-    </row>
-    <row r="5" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25"/>
-      <c r="B5" s="28" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23"/>
+      <c r="B5" s="25" t="s">
         <v>353</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="57" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27" t="s">
         <v>355</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="32" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30" t="s">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>357</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
         <v>358</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="32" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-    </row>
-    <row r="8" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28" t="s">
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23"/>
+      <c r="B8" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="26" t="s">
         <v>361</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27" t="s">
         <v>362</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="32" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="26" t="s">
         <v>364</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="D10" s="29" t="n">
+      <c r="D10" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="28" t="s">
         <v>366</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30" t="s">
+      <c r="G10" s="26"/>
+      <c r="H10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="35" t="s">
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="30" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="27" t="s">
         <v>369</v>
       </c>
-      <c r="D11" s="29" t="n">
+      <c r="D11" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>371</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
         <v>372</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="32" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30" t="s">
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="32" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30" t="s">
+      <c r="G13" s="26"/>
+      <c r="H13" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="28" t="s">
         <v>380</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="71.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="28" t="s">
         <v>383</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="26" t="s">
         <v>384</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="32" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="28" t="s">
         <v>386</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="27" t="s">
         <v>389</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="32" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="28" t="s">
         <v>390</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-    </row>
-    <row r="18" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25"/>
-      <c r="B18" s="28" t="s">
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+    </row>
+    <row r="18" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23"/>
+      <c r="B18" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="32" t="s">
+      <c r="D19" s="24"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30" t="s">
+      <c r="G19" s="26"/>
+      <c r="H19" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="26" t="s">
         <v>395</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="32" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="28" t="s">
         <v>397</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="26"/>
+      <c r="H20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="D21" s="29" t="n">
+      <c r="D21" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="28" t="s">
         <v>400</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="26" t="s">
         <v>401</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="D22" s="29" t="n">
+      <c r="D22" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="28" t="s">
         <v>403</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30" t="s">
+      <c r="G22" s="26"/>
+      <c r="H22" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="0" t="s">
         <v>404</v>
       </c>
     </row>
@@ -6855,7 +6837,7 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -6864,357 +6846,357 @@
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="32.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
         <v>405</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-    </row>
-    <row r="3" s="34" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
         <v>406</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>407</v>
       </c>
-      <c r="D3" s="29" t="n">
+      <c r="D3" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-    </row>
-    <row r="4" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25" t="s">
         <v>409</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-    </row>
-    <row r="5" s="34" customFormat="true" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="26" t="s">
         <v>410</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
         <v>411</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="32" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="35" t="s">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="30" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27" t="s">
         <v>415</v>
       </c>
-      <c r="D6" s="29" t="n">
+      <c r="D6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="28" t="s">
         <v>416</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30" t="s">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="32" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="28" t="s">
         <v>419</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="26" t="s">
         <v>420</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27" t="s">
         <v>421</v>
       </c>
-      <c r="D8" s="29" t="n">
+      <c r="D8" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="28" t="s">
         <v>422</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30" t="s">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="26" t="s">
         <v>423</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="40" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="35" t="s">
         <v>424</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="41" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="36" t="s">
         <v>425</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="35" t="s">
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="30" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="10" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23"/>
+      <c r="B10" s="25" t="s">
         <v>427</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-    </row>
-    <row r="11" s="34" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26" t="s">
         <v>428</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="41" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="32" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="28" t="s">
         <v>430</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
         <v>432</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="32" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="28" t="s">
         <v>433</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-    </row>
-    <row r="13" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25"/>
-      <c r="B13" s="28" t="s">
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23"/>
+      <c r="B13" s="25" t="s">
         <v>434</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="26" t="s">
         <v>435</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="28" t="s">
         <v>437</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="26" t="s">
         <v>438</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="27" t="s">
         <v>439</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="28" t="s">
         <v>440</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="40" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="35" t="s">
         <v>442</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="41" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="36" t="s">
         <v>443</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30" t="s">
+      <c r="G16" s="26"/>
+      <c r="H16" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="35" t="s">
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="30" t="s">
         <v>426</v>
       </c>
     </row>
@@ -7272,856 +7254,856 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="19.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="73.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="6.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="14.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="34" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="34" width="32.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="32.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
         <v>444</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="36" t="s">
         <v>446</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="42" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="37" t="s">
         <v>447</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>448</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27" t="s">
         <v>449</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="32" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="28" t="s">
         <v>450</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>451</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
         <v>452</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="32" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="28" t="s">
         <v>453</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>454</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="32" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30" t="s">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-    </row>
-    <row r="7" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25"/>
-      <c r="B7" s="28" t="s">
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23"/>
+      <c r="B7" s="25" t="s">
         <v>457</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="26" t="s">
         <v>458</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27" t="s">
         <v>459</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="32" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="28" t="s">
         <v>460</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30" t="s">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="26" t="s">
         <v>461</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="D9" s="29" t="n">
+      <c r="D9" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="28" t="s">
         <v>463</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="26" t="s">
         <v>464</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27" t="s">
         <v>465</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="32" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="28" t="s">
         <v>466</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30" t="s">
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>467</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="27" t="s">
         <v>468</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="32" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="28" t="s">
         <v>469</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>470</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
         <v>471</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="32" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="28" t="s">
         <v>472</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-    </row>
-    <row r="13" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25"/>
-      <c r="B13" s="28" t="s">
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23"/>
+      <c r="B13" s="25" t="s">
         <v>473</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="26" t="s">
         <v>474</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
         <v>475</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="28" t="s">
         <v>476</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="26" t="s">
         <v>477</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="27" t="s">
         <v>478</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="28" t="s">
         <v>479</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="27" t="s">
         <v>481</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="32" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="28" t="s">
         <v>482</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30" t="s">
+      <c r="G16" s="26"/>
+      <c r="H16" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="26" t="s">
         <v>483</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="27" t="s">
         <v>484</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="32" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="28" t="s">
         <v>485</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="26" t="s">
         <v>486</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="27" t="s">
         <v>487</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="32" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="28" t="s">
         <v>488</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30" t="s">
+      <c r="G18" s="26"/>
+      <c r="H18" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="26" t="s">
         <v>489</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="32" t="s">
+      <c r="D19" s="24"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="28" t="s">
         <v>491</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30" t="s">
+      <c r="G19" s="26"/>
+      <c r="H19" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-    </row>
-    <row r="20" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25"/>
-      <c r="B20" s="28" t="s">
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23"/>
+      <c r="B20" s="25" t="s">
         <v>492</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="26" t="s">
         <v>493</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="27" t="s">
         <v>494</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="32" t="s">
+      <c r="D21" s="24"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="28" t="s">
         <v>495</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30" t="s">
+      <c r="G21" s="26"/>
+      <c r="H21" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="26" t="s">
         <v>496</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="s">
         <v>497</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="32" t="s">
+      <c r="D22" s="24"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="28" t="s">
         <v>498</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30" t="s">
+      <c r="G22" s="26"/>
+      <c r="H22" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-    </row>
-    <row r="23" s="27" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25"/>
-      <c r="B23" s="28" t="s">
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+    </row>
+    <row r="23" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23"/>
+      <c r="B23" s="25" t="s">
         <v>499</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="93.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="26" t="s">
         <v>500</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="41" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="36" t="s">
         <v>501</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="32" t="s">
+      <c r="D24" s="24"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="28" t="s">
         <v>502</v>
       </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30" t="s">
+      <c r="G24" s="26"/>
+      <c r="H24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
     </row>
     <row r="25" customFormat="false" ht="57" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="27" t="s">
         <v>504</v>
       </c>
-      <c r="D25" s="26" t="n">
+      <c r="D25" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="28" t="s">
         <v>505</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30" t="s">
+      <c r="G25" s="26"/>
+      <c r="H25" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="26" t="s">
         <v>506</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="27" t="s">
         <v>507</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="32" t="s">
+      <c r="D26" s="24"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="28" t="s">
         <v>508</v>
       </c>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30" t="s">
+      <c r="G26" s="26"/>
+      <c r="H26" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="26" t="s">
         <v>509</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="27" t="s">
         <v>510</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="32" t="s">
+      <c r="D27" s="24"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="28" t="s">
         <v>511</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30" t="s">
+      <c r="G27" s="26"/>
+      <c r="H27" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
     </row>
     <row r="28" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="26" t="s">
         <v>512</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="27" t="s">
         <v>513</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="32" t="s">
+      <c r="D28" s="24"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="28" t="s">
         <v>514</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30" t="s">
+      <c r="G28" s="26"/>
+      <c r="H28" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="26" t="s">
         <v>515</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31" t="s">
+      <c r="B29" s="26"/>
+      <c r="C29" s="27" t="s">
         <v>516</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="32" t="s">
+      <c r="D29" s="24"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="28" t="s">
         <v>517</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30" t="s">
+      <c r="G29" s="26"/>
+      <c r="H29" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="26" t="s">
         <v>518</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31" t="s">
+      <c r="B30" s="26"/>
+      <c r="C30" s="27" t="s">
         <v>519</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="32" t="s">
+      <c r="D30" s="24"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="28" t="s">
         <v>520</v>
       </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30" t="s">
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="26" t="s">
         <v>521</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31" t="s">
+      <c r="B31" s="26"/>
+      <c r="C31" s="27" t="s">
         <v>522</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="32" t="s">
+      <c r="D31" s="24"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="28" t="s">
         <v>523</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30" t="s">
+      <c r="G31" s="26"/>
+      <c r="H31" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="26" t="s">
         <v>524</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="31" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="27" t="s">
         <v>525</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="32" t="s">
+      <c r="D32" s="24"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="28" t="s">
         <v>526</v>
       </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30" t="s">
+      <c r="G32" s="26"/>
+      <c r="H32" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="26" t="s">
         <v>527</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31" t="s">
+      <c r="B33" s="26"/>
+      <c r="C33" s="27" t="s">
         <v>528</v>
       </c>
-      <c r="D33" s="29" t="n">
+      <c r="D33" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="37" t="s">
+      <c r="E33" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="28" t="s">
         <v>529</v>
       </c>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30" t="s">
+      <c r="G33" s="26"/>
+      <c r="H33" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
     </row>
     <row r="34" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="26" t="s">
         <v>530</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="27" t="s">
         <v>531</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="32" t="s">
+      <c r="D34" s="24"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="28" t="s">
         <v>532</v>
       </c>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30" t="s">
+      <c r="G34" s="26"/>
+      <c r="H34" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="26" t="s">
         <v>533</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31" t="s">
+      <c r="B35" s="26"/>
+      <c r="C35" s="27" t="s">
         <v>534</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="32" t="s">
+      <c r="D35" s="24"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="28" t="s">
         <v>535</v>
       </c>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30" t="s">
+      <c r="G35" s="26"/>
+      <c r="H35" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
     </row>
     <row r="36" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="26" t="s">
         <v>536</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="41" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="36" t="s">
         <v>537</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="32" t="s">
+      <c r="D36" s="24"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="28" t="s">
         <v>538</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30" t="s">
+      <c r="G36" s="26"/>
+      <c r="H36" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="26" t="s">
         <v>539</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31" t="s">
+      <c r="B37" s="26"/>
+      <c r="C37" s="27" t="s">
         <v>540</v>
       </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="32" t="s">
+      <c r="D37" s="24"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="28" t="s">
         <v>541</v>
       </c>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30" t="s">
+      <c r="G37" s="26"/>
+      <c r="H37" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
     </row>
     <row r="38" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="26" t="s">
         <v>542</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="31" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="27" t="s">
         <v>543</v>
       </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="32" t="s">
+      <c r="D38" s="24"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="28" t="s">
         <v>544</v>
       </c>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30" t="s">
+      <c r="G38" s="26"/>
+      <c r="H38" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
     </row>
     <row r="39" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="26" t="s">
         <v>545</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="27" t="s">
         <v>546</v>
       </c>
-      <c r="D39" s="29" t="n">
+      <c r="D39" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E39" s="37" t="s">
+      <c r="E39" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="28" t="s">
         <v>547</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30" t="s">
+      <c r="G39" s="26"/>
+      <c r="H39" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="26" t="s">
         <v>548</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="31" t="s">
+      <c r="B40" s="26"/>
+      <c r="C40" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="32" t="s">
+      <c r="D40" s="24"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="28" t="s">
         <v>550</v>
       </c>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30" t="s">
+      <c r="G40" s="26"/>
+      <c r="H40" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
     </row>
   </sheetData>
   <autoFilter ref="H1:H40">
@@ -8176,148 +8158,148 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="43" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="71.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="43" width="25.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="43" width="6.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="43" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="43" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="71.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="25.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="6.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="38" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="39" t="s">
         <v>551</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="40" t="s">
         <v>552</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="41" t="s">
         <v>553</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="42" t="s">
         <v>554</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="43" t="s">
         <v>555</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="44" t="s">
         <v>556</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="45" t="s">
         <v>557</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="46" t="s">
         <v>558</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="47" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="48" t="s">
         <v>560</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55" t="n">
+      <c r="C4" s="49"/>
+      <c r="D4" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="51" t="s">
         <v>561</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55" t="n">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="49"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="52" t="s">
         <v>562</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="55" t="n">
+      <c r="C6" s="49"/>
+      <c r="D6" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="54"/>
+      <c r="E6" s="49"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="51" t="s">
         <v>563</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55" t="n">
+      <c r="C7" s="49"/>
+      <c r="D7" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="54"/>
+      <c r="E7" s="49"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="51" t="s">
         <v>564</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55" t="n">
+      <c r="C8" s="49"/>
+      <c r="D8" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="54"/>
+      <c r="E8" s="49"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="51" t="s">
         <v>565</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55" t="n">
+      <c r="C9" s="49"/>
+      <c r="D9" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="54"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="51" t="s">
         <v>566</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55" t="n">
+      <c r="C10" s="49"/>
+      <c r="D10" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="54"/>
+      <c r="E10" s="49"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="D11" s="59" t="n">
+      <c r="D11" s="54" t="n">
         <f aca="false">SUM(D4:D10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="38" t="s">
         <v>568</v>
       </c>
-      <c r="D12" s="60" t="n">
+      <c r="D12" s="55" t="n">
         <f aca="false">COUNT(D4:D10)</f>
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="38" t="s">
         <v>569</v>
       </c>
-      <c r="D13" s="61" t="n">
+      <c r="D13" s="56" t="n">
         <f aca="false">IFERROR(D11/(D12*2), 0)</f>
         <v>0</v>
       </c>
@@ -8358,149 +8340,149 @@
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="32.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
         <v>570</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-    </row>
-    <row r="3" s="34" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
         <v>571</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>572</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="31" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="27" t="s">
         <v>573</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>574</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="62" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="57" t="s">
         <v>575</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="31" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="27" t="s">
         <v>576</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>577</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
         <v>578</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="31" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="27" t="s">
         <v>579</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>580</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27" t="s">
         <v>581</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="31" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="27" t="s">
         <v>582</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30" t="s">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
   </sheetData>
   <autoFilter ref="H1:H6"/>

</xml_diff>

<commit_message>
Copy new "psm-IP-*" reqs from RTM.org to RTM.xlsx
This is a work in progress.  The new reqs we added in RTM.org under
the "psm-IP-*" names ("IP" for "In Progress") are now also in
RTM.xlsx, in the new sheet "Development and Maintenance", where they
all have the same numbers but with a "psm-DM-*" prefix instead.

However, not all of these are actually development and maintenance
requirements.  A separate commit will move and rename some of them to
more appropriate sheets.

Also, psm-IP-3.7 (the new "FOR FUTURE FEATURES" requirement) needs to
get broken out into separate requirements based on the issues
associated with it.  That will also be in a separate commit.
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FUNC Reqs" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,9 +14,10 @@
     <sheet name="Information Architecture" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Integration and Utility" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Access and Delivery" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Performance" sheetId="7" state="hidden" r:id="rId8"/>
-    <sheet name="Pharmacy (MMIS)" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Selections" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Development and Maintenance" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Performance" sheetId="8" state="hidden" r:id="rId9"/>
+    <sheet name="Pharmacy (MMIS)" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Selections" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Access and Delivery'!$H$1:$H$40</definedName>
@@ -24,7 +25,7 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Information Architecture'!$H$1:$H$23</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Integration and Utility'!$H$1:$H$16</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Intermediary &amp; Interface'!$H$1:$H$17</definedName>
-    <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'Pharmacy (MMIS)'!$H$1:$H$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'Pharmacy (MMIS)'!$H$1:$H$6</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Standards and Conditions'!$H$1:$H$14</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="612">
   <si>
     <t xml:space="preserve">Requirement ID Number</t>
   </si>
@@ -2138,6 +2139,90 @@
   </si>
   <si>
     <t xml:space="preserve">TA.SP.74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall have an open source repository and source code base organized to be welcoming to outside contributors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall include and undergo automated testing at regular intervals, through continuous integration and deployment processes.  The PSM shall also undergo manual testing and QA as needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall use modern source code dependency management techniques, and shall use up-to-date versions of upstream third-party dependencies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall use documented build, test, release, and installation processes that are automated as much as possible, for both development and production use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall use D.R.Y. coding principles to avoid unnecessary complexity, inflexibility, redundancy, and denormalization in the source code and database schemas, and to use precise terminology in data structures and operations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall use system resources efficiently and in proportion to operational demands and data size.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall be configurable where feasible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall be secure from unauthorized access or use, and shall sanitize inputs and outputs where possible so as to avoid compromising itself or other systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall be accessible in compliance with Section 508 of the Rehabilitation Act.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM's user interface shall be as simple, comprehensible, navigable, reliable, robust in the face of error, and responsive as possible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall support searching and pattern-matching based on all fields accepted as input (and based on all reasonable combinations of such fields).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall have the ability to enforce limits on the number of providers of a given type enrolled simultaneously.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall support admin-configurable automated re-screening.  C.f. psm-FR-7.3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-DM-3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PSM shall support provider agents (a.k.a. service agents a.k.a. non-provider users) who act on a provider's behalf and whose authorization may be a subset of that provider's.</t>
   </si>
   <si>
     <t xml:space="preserve">Means of demonstrating compliance ---&gt;</t>
@@ -2520,7 +2605,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2671,6 +2756,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -2862,9 +2963,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1913400</xdr:colOff>
+      <xdr:colOff>1913040</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2874,7 +2975,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="634680" y="0"/>
-          <a:ext cx="1913400" cy="675720"/>
+          <a:ext cx="1913040" cy="675360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2929,10 +3030,10 @@
   </sheetPr>
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5490,6 +5591,100 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>611</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -5498,9 +5693,9 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7249,7 +7444,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8121,16 +8316,16 @@
     <mergeCell ref="B23:C23"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E6 E8:E40" type="list">
-      <formula1>Selections!$B$4:$B$6</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D40" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:H6 H8:H12 H14:H19 H21:H22 H24:H40" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E6 E8:E40" type="list">
+      <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -8150,6 +8345,344 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="66.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="38" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="24"/>
+      <c r="F1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>551</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="36" t="s">
+        <v>552</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+    </row>
+    <row r="3" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
+        <v>553</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
+        <v>554</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27" t="s">
+        <v>556</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
+        <v>558</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+    </row>
+    <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27" t="s">
+        <v>560</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26" t="s">
+        <v>561</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
+        <v>562</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27" t="s">
+        <v>564</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26" t="s">
+        <v>565</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27" t="s">
+        <v>566</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27" t="s">
+        <v>568</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26" t="s">
+        <v>569</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+    </row>
+    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26" t="s">
+        <v>571</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
+        <v>572</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="26" t="s">
+        <v>573</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="s">
+        <v>574</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+    </row>
+    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
+        <v>575</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
+        <v>576</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="15" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="26" t="s">
+        <v>577</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27" t="s">
+        <v>578</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D15" type="list">
+      <formula1>Selections!$A$4:$A$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H15" type="list">
+      <formula1>Selections!$C$4:$C$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E15" type="list">
+      <formula1>Selections!$B$4:$B$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -8158,148 +8691,148 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="71.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="25.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="6.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="38" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="42" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="71.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="42" width="25.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="42" width="6.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="42" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="42" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1" s="39" t="s">
-        <v>551</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>552</v>
-      </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="C1" s="43" t="s">
+        <v>579</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>580</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="41" t="s">
-        <v>553</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>554</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>555</v>
-      </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
+      <c r="B2" s="45" t="s">
+        <v>581</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>582</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>583</v>
+      </c>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="44" t="s">
-        <v>556</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>557</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>558</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>559</v>
+      <c r="B3" s="48" t="s">
+        <v>584</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>585</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="48" t="s">
-        <v>560</v>
-      </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50" t="n">
+      <c r="B4" s="52" t="s">
+        <v>588</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50" t="n">
+      <c r="B5" s="55" t="s">
+        <v>589</v>
+      </c>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="52" t="s">
-        <v>562</v>
-      </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50" t="n">
+      <c r="B6" s="56" t="s">
+        <v>590</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="49"/>
+      <c r="E6" s="53"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="51" t="s">
-        <v>563</v>
-      </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50" t="n">
+      <c r="B7" s="55" t="s">
+        <v>591</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="49"/>
+      <c r="E7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="51" t="s">
-        <v>564</v>
-      </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50" t="n">
+      <c r="B8" s="55" t="s">
+        <v>592</v>
+      </c>
+      <c r="C8" s="53"/>
+      <c r="D8" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="49"/>
+      <c r="E8" s="53"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="51" t="s">
-        <v>565</v>
-      </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50" t="n">
+      <c r="B9" s="55" t="s">
+        <v>593</v>
+      </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="49"/>
+      <c r="E9" s="53"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="51" t="s">
-        <v>566</v>
-      </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50" t="n">
+      <c r="B10" s="55" t="s">
+        <v>594</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="49"/>
+      <c r="E10" s="53"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="53" t="s">
-        <v>567</v>
-      </c>
-      <c r="D11" s="54" t="n">
+      <c r="C11" s="57" t="s">
+        <v>595</v>
+      </c>
+      <c r="D11" s="58" t="n">
         <f aca="false">SUM(D4:D10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="38" t="s">
-        <v>568</v>
-      </c>
-      <c r="D12" s="55" t="n">
+      <c r="C12" s="42" t="s">
+        <v>596</v>
+      </c>
+      <c r="D12" s="59" t="n">
         <f aca="false">COUNT(D4:D10)</f>
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="38" t="s">
-        <v>569</v>
-      </c>
-      <c r="D13" s="56" t="n">
+      <c r="C13" s="42" t="s">
+        <v>597</v>
+      </c>
+      <c r="D13" s="60" t="n">
         <f aca="false">IFERROR(D11/(D12*2), 0)</f>
         <v>0</v>
       </c>
@@ -8326,7 +8859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8388,7 +8921,7 @@
     <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="23"/>
       <c r="B2" s="25" t="s">
-        <v>570</v>
+        <v>598</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="24"/>
@@ -8402,16 +8935,16 @@
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>571</v>
+        <v>599</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="27" t="s">
-        <v>572</v>
+        <v>600</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
       <c r="F3" s="27" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26" t="s">
@@ -8423,16 +8956,16 @@
     </row>
     <row r="4" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>574</v>
+        <v>602</v>
       </c>
       <c r="B4" s="26"/>
-      <c r="C4" s="57" t="s">
-        <v>575</v>
+      <c r="C4" s="61" t="s">
+        <v>603</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="27" t="s">
-        <v>576</v>
+        <v>604</v>
       </c>
       <c r="G4" s="26"/>
       <c r="H4" s="26" t="s">
@@ -8444,16 +8977,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>577</v>
+        <v>605</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="27" t="s">
-        <v>578</v>
+        <v>606</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="27" t="s">
-        <v>579</v>
+        <v>607</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26" t="s">
@@ -8465,16 +8998,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>580</v>
+        <v>608</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="27" t="s">
-        <v>581</v>
+        <v>609</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="27" t="s">
-        <v>582</v>
+        <v>610</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
@@ -8512,98 +9045,4 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A3:C10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
-        <v>374</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
"Development and Maintenance" -> "Software Quality"
Rename the new sheet created in commit 9ba5431bf, and change the
"psm-DM-" prefix to "psm-SQ-" accordingly.
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Information Architecture" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Integration and Utility" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Access and Delivery" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Development and Maintenance" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Software Quality" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Performance" sheetId="8" state="hidden" r:id="rId9"/>
     <sheet name="Pharmacy (MMIS)" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Selections" sheetId="10" state="visible" r:id="rId11"/>
@@ -2141,85 +2141,85 @@
     <t xml:space="preserve">TA.SP.74</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-1.1</t>
+    <t xml:space="preserve">psm-SQ-1.1</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall have an open source repository and source code base organized to be welcoming to outside contributors.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-1.2</t>
+    <t xml:space="preserve">psm-SQ-1.2</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall include and undergo automated testing at regular intervals, through continuous integration and deployment processes.  The PSM shall also undergo manual testing and QA as needed.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-1.3</t>
+    <t xml:space="preserve">psm-SQ-1.3</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall use modern source code dependency management techniques, and shall use up-to-date versions of upstream third-party dependencies.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-1.4</t>
+    <t xml:space="preserve">psm-SQ-1.4</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall use documented build, test, release, and installation processes that are automated as much as possible, for both development and production use.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-1.5</t>
+    <t xml:space="preserve">psm-SQ-1.5</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall use D.R.Y. coding principles to avoid unnecessary complexity, inflexibility, redundancy, and denormalization in the source code and database schemas, and to use precise terminology in data structures and operations.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-1.6</t>
+    <t xml:space="preserve">psm-SQ-1.6</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall use system resources efficiently and in proportion to operational demands and data size.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-2.1</t>
+    <t xml:space="preserve">psm-SQ-2.1</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall be configurable where feasible.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-2.3</t>
+    <t xml:space="preserve">psm-SQ-2.3</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall be secure from unauthorized access or use, and shall sanitize inputs and outputs where possible so as to avoid compromising itself or other systems.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-3.1</t>
+    <t xml:space="preserve">psm-SQ-3.1</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall be accessible in compliance with Section 508 of the Rehabilitation Act.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-3.2</t>
+    <t xml:space="preserve">psm-SQ-3.2</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM's user interface shall be as simple, comprehensible, navigable, reliable, robust in the face of error, and responsive as possible.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-3.3</t>
+    <t xml:space="preserve">psm-SQ-3.3</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall support searching and pattern-matching based on all fields accepted as input (and based on all reasonable combinations of such fields).</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-3.4</t>
+    <t xml:space="preserve">psm-SQ-3.4</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall have the ability to enforce limits on the number of providers of a given type enrolled simultaneously.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-3.5</t>
+    <t xml:space="preserve">psm-SQ-3.5</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall support admin-configurable automated re-screening.  C.f. psm-FR-7.3.</t>
   </si>
   <si>
-    <t xml:space="preserve">psm-DM-3.6</t>
+    <t xml:space="preserve">psm-SQ-3.6</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall support provider agents (a.k.a. service agents a.k.a. non-provider users) who act on a provider's behalf and whose authorization may be a subset of that provider's.</t>
@@ -5693,7 +5693,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
@@ -8348,7 +8348,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Unhide all rows in all tabs in the RTM
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="FUNC Reqs" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="614">
   <si>
     <t xml:space="preserve">Requirement ID Number</t>
   </si>
@@ -1502,6 +1502,9 @@
   </si>
   <si>
     <t xml:space="preserve">4.  S&amp;C:  Modularity Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psm-SA-4.0</t>
   </si>
   <si>
     <t xml:space="preserve">The PSM shall use regionally standardized business rule definitions in both human and machine-readable formats.</t>
@@ -2615,7 +2618,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2724,10 +2727,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2741,10 +2740,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2781,18 +2776,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2979,7 +2962,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2996,8 +2979,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="634680" y="0"/>
-          <a:ext cx="1913040" cy="675360"/>
+          <a:off x="635400" y="0"/>
+          <a:ext cx="1912320" cy="675360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3052,10 +3035,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
+      <selection pane="bottomLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8348,7 +8331,7 @@
       </c>
       <c r="D95" s="22"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="27" t="s">
+      <c r="F95" s="21" t="s">
         <v>174</v>
       </c>
       <c r="G95" s="20"/>
@@ -9380,11 +9363,11 @@
       </c>
       <c r="D96" s="22"/>
       <c r="E96" s="23"/>
-      <c r="F96" s="27" t="s">
+      <c r="F96" s="21" t="s">
         <v>174</v>
       </c>
       <c r="G96" s="20"/>
-      <c r="H96" s="28" t="s">
+      <c r="H96" s="27" t="s">
         <v>49</v>
       </c>
       <c r="I96" s="20"/>
@@ -10688,8 +10671,8 @@
       <c r="C110" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="D110" s="29"/>
-      <c r="E110" s="29"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="28"/>
       <c r="F110" s="7" t="s">
         <v>14</v>
       </c>
@@ -10713,11 +10696,11 @@
       </c>
       <c r="D111" s="22"/>
       <c r="E111" s="23"/>
-      <c r="F111" s="27" t="s">
+      <c r="F111" s="21" t="s">
         <v>174</v>
       </c>
       <c r="G111" s="20"/>
-      <c r="H111" s="28" t="s">
+      <c r="H111" s="27" t="s">
         <v>49</v>
       </c>
       <c r="I111" s="20"/>
@@ -11752,35 +11735,35 @@
     <mergeCell ref="B109:C109"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E8 E10:E29 E31:E47 E54 E56:E60 E65:E72 E74:E81 E83:E94 E98:E100 E102 E104:E108 E110" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E8 E10:E29 E31:E47 E54 E56:E60 E65:E72 E74:E81 E83:E94 E98:E100 E102 E104:E108 E110" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D61:D63 D95:D96 D111" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D8 D10:D29 D31:D47 D54 D56:D60 D65:D72 D74:D81 D83:D94 D98:D100 D102 D104:D108 D110" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H61:H63 H95:H96 H111" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5 H7 H12 H16:H17 H19:H23 H26:H28 H40:H41 H43:H44 H46:H53 H74 H78 H83:H85 H92 H94 H98:H102 H104:H107 H110" type="list">
+      <formula1>$C$5:$C$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4 H6 H8 H10:H11 H13:H15 H18 H24:H25 H29 H34 H42 H45 H54 H60 H66:H67 H86:H91 H93 H108" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E61:E63 E95:E96 E111" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H31:H33 H35:H39 H56:H59 H65 H68:H72 H75:H77 H79:H81" type="list">
+      <formula1>Selections!$C$5:$C$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D61:D63 D95:D96 D111" type="list">
+      <formula1>Selections!$A$4:$A$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E61:E63 E95:E96 E111" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5 H7 H12 H16:H17 H19:H23 H26:H28 H40:H41 H43:H44 H46:H53 H74 H78 H83:H85 H92 H94 H98:H102 H104:H107 H110" type="list">
-      <formula1>$C$5:$C$6</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D8 D10:D29 D31:D47 D54 D56:D60 D65:D72 D74:D81 D83:D94 D98:D100 D102 D104:D108 D110" type="list">
-      <formula1>Selections!$A$4:$A$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H31:H33 H35:H39 H56:H59 H65 H68:H72 H75:H77 H79:H81" type="list">
-      <formula1>Selections!$C$5:$C$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4 H6 H8 H10:H11 H13:H15 H18 H24:H25 H29 H34 H42 H45 H54 H60 H66:H67 H86:H91 H93 H108" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H61:H63 H95:H96 H111" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11845,7 +11828,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
@@ -11907,7 +11890,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -11948,10 +11931,10 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
@@ -11983,11 +11966,11 @@
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="9"/>
       <c r="E2" s="22"/>
       <c r="F2" s="7"/>
@@ -12002,7 +11985,7 @@
         <v>283</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="24" t="s">
         <v>284</v>
       </c>
       <c r="D3" s="9" t="n">
@@ -12011,7 +11994,7 @@
       <c r="E3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="31" t="s">
         <v>285</v>
       </c>
       <c r="G3" s="20"/>
@@ -12023,11 +12006,11 @@
       <c r="K3" s="20"/>
     </row>
     <row r="4" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30" t="s">
         <v>286</v>
       </c>
-      <c r="C4" s="31"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="9"/>
       <c r="E4" s="20"/>
       <c r="F4" s="7"/>
@@ -12042,12 +12025,12 @@
         <v>287</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="24" t="s">
         <v>288</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="31" t="s">
         <v>289</v>
       </c>
       <c r="G5" s="20"/>
@@ -12056,7 +12039,7 @@
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="32" t="s">
         <v>290</v>
       </c>
     </row>
@@ -12065,12 +12048,12 @@
         <v>291</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="24" t="s">
         <v>292</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="20"/>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="31" t="s">
         <v>293</v>
       </c>
       <c r="G6" s="20"/>
@@ -12086,7 +12069,7 @@
         <v>294</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="24" t="s">
         <v>295</v>
       </c>
       <c r="D7" s="9" t="n">
@@ -12095,7 +12078,7 @@
       <c r="E7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="31" t="s">
         <v>296</v>
       </c>
       <c r="G7" s="20"/>
@@ -12113,12 +12096,12 @@
         <v>298</v>
       </c>
       <c r="B8" s="20"/>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="24" t="s">
         <v>299</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="31" t="s">
         <v>300</v>
       </c>
       <c r="G8" s="20"/>
@@ -12134,12 +12117,12 @@
         <v>301</v>
       </c>
       <c r="B9" s="20"/>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="24" t="s">
         <v>302</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="31" t="s">
         <v>303</v>
       </c>
       <c r="G9" s="20"/>
@@ -12148,16 +12131,16 @@
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="33" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30" t="s">
         <v>305</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="9"/>
       <c r="E10" s="20"/>
       <c r="F10" s="7"/>
@@ -12172,12 +12155,12 @@
         <v>306</v>
       </c>
       <c r="B11" s="20"/>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="24" t="s">
         <v>307</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="31" t="s">
         <v>308</v>
       </c>
       <c r="G11" s="20"/>
@@ -12193,12 +12176,12 @@
         <v>309</v>
       </c>
       <c r="B12" s="20"/>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="24" t="s">
         <v>310</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="31" t="s">
         <v>311</v>
       </c>
       <c r="G12" s="20"/>
@@ -12207,16 +12190,16 @@
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="32" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="13" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="22"/>
       <c r="E13" s="20"/>
       <c r="F13" s="7"/>
@@ -12231,12 +12214,12 @@
         <v>314</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="24" t="s">
         <v>315</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="31" t="s">
         <v>316</v>
       </c>
       <c r="G14" s="20"/>
@@ -12252,12 +12235,12 @@
         <v>317</v>
       </c>
       <c r="B15" s="20"/>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="24" t="s">
         <v>318</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="31" t="s">
         <v>319</v>
       </c>
       <c r="G15" s="20"/>
@@ -12273,7 +12256,7 @@
         <v>320</v>
       </c>
       <c r="B16" s="20"/>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="24" t="s">
         <v>321</v>
       </c>
       <c r="D16" s="9" t="n">
@@ -12282,7 +12265,7 @@
       <c r="E16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="31" t="s">
         <v>322</v>
       </c>
       <c r="G16" s="22"/>
@@ -12291,14 +12274,14 @@
       </c>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
-      <c r="K16" s="36"/>
+      <c r="K16" s="34"/>
     </row>
     <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
         <v>323</v>
       </c>
       <c r="B17" s="20"/>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="24" t="s">
         <v>324</v>
       </c>
       <c r="D17" s="9" t="n">
@@ -12307,7 +12290,7 @@
       <c r="E17" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="31" t="s">
         <v>322</v>
       </c>
       <c r="G17" s="22"/>
@@ -12316,14 +12299,14 @@
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
-      <c r="K17" s="36"/>
+      <c r="K17" s="34"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B18" s="20"/>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="24" t="s">
         <v>326</v>
       </c>
       <c r="D18" s="22"/>
@@ -12348,19 +12331,19 @@
     <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E17" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D18" type="list">
+      <formula1>Selections!$A$4:$A$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E17" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D18" type="list">
-      <formula1>Selections!$A$4:$A$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5:H9 H11:H12 H14:H18" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5:H9 H11:H12 H14:H18" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E18" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E18" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12384,7 +12367,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12401,10 +12384,10 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
@@ -12435,12 +12418,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="7"/>
@@ -12450,17 +12433,17 @@
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
         <v>328</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="33" t="s">
         <v>329</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="35" t="s">
         <v>330</v>
       </c>
       <c r="G3" s="20"/>
@@ -12471,12 +12454,12 @@
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31" t="s">
+    <row r="4" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="C4" s="31"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
       <c r="F4" s="7"/>
@@ -12486,35 +12469,35 @@
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
         <v>332</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>333</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="31" t="s">
         <v>334</v>
       </c>
       <c r="G5" s="20"/>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="36" t="s">
         <v>94</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="33" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31" t="s">
+    <row r="6" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="C6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
       <c r="F6" s="7"/>
@@ -12529,12 +12512,12 @@
         <v>337</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="33" t="s">
         <v>338</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="31" t="s">
         <v>339</v>
       </c>
       <c r="G7" s="20"/>
@@ -12547,12 +12530,12 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31" t="s">
+    <row r="8" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="C8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="22"/>
       <c r="E8" s="23"/>
       <c r="F8" s="7"/>
@@ -12562,31 +12545,33 @@
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" s="4" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32" t="s">
+    <row r="9" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34" t="s">
         <v>342</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="24" t="s">
+        <v>343</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
-      <c r="F9" s="39" t="s">
-        <v>343</v>
+      <c r="F9" s="37" t="s">
+        <v>344</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
-      <c r="K9" s="30" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="10" s="4" customFormat="true" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K9" s="29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32" t="s">
         <v>346</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24" t="s">
+        <v>347</v>
       </c>
       <c r="D10" s="9" t="n">
         <v>2</v>
@@ -12594,7 +12579,7 @@
       <c r="E10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="31" t="s">
         <v>322</v>
       </c>
       <c r="G10" s="22"/>
@@ -12603,17 +12588,17 @@
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
-      <c r="K10" s="36" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="11" s="4" customFormat="true" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K10" s="34" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>348</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32" t="s">
         <v>349</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="24" t="s">
+        <v>350</v>
       </c>
       <c r="D11" s="9" t="n">
         <v>2</v>
@@ -12621,8 +12606,8 @@
       <c r="E11" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="33" t="s">
-        <v>350</v>
+      <c r="F11" s="31" t="s">
+        <v>351</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="20" t="s">
@@ -12630,22 +12615,22 @@
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
-      <c r="K11" s="36" t="s">
-        <v>347</v>
+      <c r="K11" s="34" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>351</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="32" t="s">
         <v>352</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="24" t="s">
+        <v>353</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="33" t="s">
-        <v>353</v>
+      <c r="F12" s="31" t="s">
+        <v>354</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="20" t="s">
@@ -12657,11 +12642,11 @@
     </row>
     <row r="13" s="4" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>354</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32" t="s">
         <v>355</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="24" t="s">
+        <v>356</v>
       </c>
       <c r="D13" s="9" t="n">
         <v>1</v>
@@ -12669,8 +12654,8 @@
       <c r="E13" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="33" t="s">
-        <v>356</v>
+      <c r="F13" s="31" t="s">
+        <v>357</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="20" t="s">
@@ -12682,16 +12667,16 @@
     </row>
     <row r="14" s="4" customFormat="true" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>357</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32" t="s">
         <v>358</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="24" t="s">
+        <v>359</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="33" t="s">
-        <v>359</v>
+      <c r="F14" s="31" t="s">
+        <v>360</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="20" t="s">
@@ -12716,16 +12701,16 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5 H7 H10:H14" type="list">
-      <formula1>Selections!$C$4:$C$9</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E14" type="list">
+      <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D14" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E14" type="list">
-      <formula1>Selections!$B$4:$B$6</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5 H7 H10:H14" type="list">
+      <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -12747,8 +12732,8 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12765,10 +12750,10 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
@@ -12799,12 +12784,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31" t="s">
-        <v>360</v>
-      </c>
-      <c r="C2" s="31"/>
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" s="30"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="7"/>
@@ -12814,18 +12799,18 @@
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="32" t="s">
-        <v>362</v>
+      <c r="C3" s="24" t="s">
+        <v>363</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="37" t="s">
-        <v>363</v>
+      <c r="F3" s="35" t="s">
+        <v>364</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -12834,21 +12819,21 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B4" s="20"/>
-      <c r="C4" s="32" t="s">
-        <v>366</v>
+      <c r="C4" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="F4" s="33" t="s">
-        <v>367</v>
+      <c r="F4" s="31" t="s">
+        <v>368</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
@@ -12858,12 +12843,12 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31" t="s">
-        <v>368</v>
-      </c>
-      <c r="C5" s="31"/>
+    <row r="5" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
       <c r="F5" s="7"/>
@@ -12873,18 +12858,18 @@
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" customFormat="false" ht="57" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="32" t="s">
-        <v>370</v>
+      <c r="C6" s="24" t="s">
+        <v>371</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="33" t="s">
-        <v>371</v>
+      <c r="F6" s="31" t="s">
+        <v>372</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">
@@ -12894,18 +12879,18 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="32" t="s">
-        <v>373</v>
+      <c r="C7" s="24" t="s">
+        <v>374</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="33" t="s">
-        <v>374</v>
+      <c r="F7" s="31" t="s">
+        <v>375</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20" t="s">
@@ -12915,12 +12900,12 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31" t="s">
-        <v>375</v>
-      </c>
-      <c r="C8" s="31"/>
+    <row r="8" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30" t="s">
+        <v>376</v>
+      </c>
+      <c r="C8" s="30"/>
       <c r="D8" s="22"/>
       <c r="E8" s="23"/>
       <c r="F8" s="7"/>
@@ -12930,18 +12915,18 @@
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B9" s="20"/>
-      <c r="C9" s="32" t="s">
-        <v>377</v>
+      <c r="C9" s="24" t="s">
+        <v>378</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
-      <c r="F9" s="33" t="s">
-        <v>378</v>
+      <c r="F9" s="31" t="s">
+        <v>379</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
@@ -12951,13 +12936,13 @@
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B10" s="20"/>
-      <c r="C10" s="32" t="s">
-        <v>380</v>
+      <c r="C10" s="24" t="s">
+        <v>381</v>
       </c>
       <c r="D10" s="9" t="n">
         <v>1</v>
@@ -12965,8 +12950,8 @@
       <c r="E10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>381</v>
+      <c r="F10" s="31" t="s">
+        <v>382</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20" t="s">
@@ -12974,17 +12959,17 @@
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
-      <c r="K10" s="35" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K10" s="33" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B11" s="20"/>
-      <c r="C11" s="32" t="s">
-        <v>384</v>
+      <c r="C11" s="24" t="s">
+        <v>385</v>
       </c>
       <c r="D11" s="9" t="n">
         <v>1</v>
@@ -12992,8 +12977,8 @@
       <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="33" t="s">
-        <v>385</v>
+      <c r="F11" s="31" t="s">
+        <v>386</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
@@ -13003,18 +12988,18 @@
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B12" s="20"/>
-      <c r="C12" s="32" t="s">
-        <v>387</v>
+      <c r="C12" s="24" t="s">
+        <v>388</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="33" t="s">
-        <v>388</v>
+      <c r="F12" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20" t="s">
@@ -13023,21 +13008,21 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B13" s="20"/>
-      <c r="C13" s="32" t="s">
-        <v>391</v>
+      <c r="C13" s="24" t="s">
+        <v>392</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="33" t="s">
-        <v>392</v>
+      <c r="F13" s="31" t="s">
+        <v>393</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20" t="s">
@@ -13047,18 +13032,18 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="32" t="s">
-        <v>394</v>
+      <c r="C14" s="24" t="s">
+        <v>395</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="33" t="s">
-        <v>395</v>
+      <c r="F14" s="31" t="s">
+        <v>396</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20" t="s">
@@ -13068,18 +13053,18 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" customFormat="false" ht="71.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="71.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B15" s="20"/>
-      <c r="C15" s="32" t="s">
-        <v>397</v>
+      <c r="C15" s="24" t="s">
+        <v>398</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="33" t="s">
-        <v>398</v>
+      <c r="F15" s="31" t="s">
+        <v>399</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20" t="s">
@@ -13089,21 +13074,21 @@
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B16" s="20"/>
-      <c r="C16" s="32" t="s">
-        <v>400</v>
+      <c r="C16" s="24" t="s">
+        <v>401</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="33" t="s">
-        <v>401</v>
+      <c r="F16" s="31" t="s">
+        <v>402</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>108</v>
@@ -13112,18 +13097,18 @@
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B17" s="20"/>
-      <c r="C17" s="32" t="s">
-        <v>404</v>
+      <c r="C17" s="24" t="s">
+        <v>405</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="33" t="s">
-        <v>405</v>
+      <c r="F17" s="31" t="s">
+        <v>406</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20" t="s">
@@ -13133,12 +13118,12 @@
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31" t="s">
-        <v>406</v>
-      </c>
-      <c r="C18" s="31"/>
+    <row r="18" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="29"/>
+      <c r="B18" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="C18" s="30"/>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
       <c r="F18" s="7"/>
@@ -13150,16 +13135,16 @@
     </row>
     <row r="19" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B19" s="20"/>
-      <c r="C19" s="32" t="s">
-        <v>408</v>
+      <c r="C19" s="24" t="s">
+        <v>409</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="33" t="s">
-        <v>409</v>
+      <c r="F19" s="31" t="s">
+        <v>410</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20" t="s">
@@ -13169,18 +13154,18 @@
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B20" s="20"/>
-      <c r="C20" s="32" t="s">
-        <v>411</v>
+      <c r="C20" s="24" t="s">
+        <v>412</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="33" t="s">
-        <v>412</v>
+      <c r="F20" s="31" t="s">
+        <v>413</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20" t="s">
@@ -13190,13 +13175,13 @@
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B21" s="20"/>
-      <c r="C21" s="32" t="s">
-        <v>414</v>
+      <c r="C21" s="24" t="s">
+        <v>415</v>
       </c>
       <c r="D21" s="9" t="n">
         <v>4</v>
@@ -13204,11 +13189,11 @@
       <c r="E21" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="33" t="s">
-        <v>415</v>
+      <c r="F21" s="31" t="s">
+        <v>416</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H21" s="20" t="s">
         <v>21</v>
@@ -13217,13 +13202,13 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B22" s="20"/>
-      <c r="C22" s="32" t="s">
-        <v>417</v>
+      <c r="C22" s="24" t="s">
+        <v>418</v>
       </c>
       <c r="D22" s="9" t="n">
         <v>4</v>
@@ -13231,8 +13216,8 @@
       <c r="E22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="33" t="s">
-        <v>418</v>
+      <c r="F22" s="31" t="s">
+        <v>419</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20" t="s">
@@ -13242,9 +13227,9 @@
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G23" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -13262,16 +13247,16 @@
     <mergeCell ref="B18:C18"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:H4 H6:H7 H9:H17 H19:H22" type="list">
-      <formula1>Selections!$C$4:$C$9</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D22" type="list">
+      <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E22" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E22" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D22" type="list">
-      <formula1>Selections!$A$4:$A$7</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:H4 H6:H7 H9:H17 H19:H22" type="list">
+      <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -13294,9 +13279,9 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13313,10 +13298,10 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
@@ -13347,12 +13332,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31" t="s">
-        <v>420</v>
-      </c>
-      <c r="C2" s="31"/>
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" s="30"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="7"/>
@@ -13362,13 +13347,13 @@
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="32" t="s">
-        <v>422</v>
+      <c r="C3" s="24" t="s">
+        <v>423</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>1</v>
@@ -13376,8 +13361,8 @@
       <c r="E3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>423</v>
+      <c r="F3" s="31" t="s">
+        <v>424</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -13387,12 +13372,12 @@
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31" t="s">
-        <v>424</v>
-      </c>
-      <c r="C4" s="31"/>
+    <row r="4" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4" s="30"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="7"/>
@@ -13402,18 +13387,18 @@
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="32" t="s">
-        <v>426</v>
+      <c r="C5" s="24" t="s">
+        <v>427</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="33" t="s">
-        <v>427</v>
+      <c r="F5" s="31" t="s">
+        <v>428</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
@@ -13421,17 +13406,17 @@
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="35" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="33" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="32" t="s">
-        <v>430</v>
+      <c r="C6" s="24" t="s">
+        <v>431</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>2</v>
@@ -13439,8 +13424,8 @@
       <c r="E6" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>431</v>
+      <c r="F6" s="31" t="s">
+        <v>432</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">
@@ -13450,18 +13435,18 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="32" t="s">
-        <v>433</v>
+      <c r="C7" s="24" t="s">
+        <v>434</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="33" t="s">
-        <v>434</v>
+      <c r="F7" s="31" t="s">
+        <v>435</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20" t="s">
@@ -13471,13 +13456,13 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B8" s="20"/>
-      <c r="C8" s="32" t="s">
-        <v>436</v>
+      <c r="C8" s="24" t="s">
+        <v>437</v>
       </c>
       <c r="D8" s="9" t="n">
         <v>3</v>
@@ -13485,8 +13470,8 @@
       <c r="E8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>437</v>
+      <c r="F8" s="31" t="s">
+        <v>438</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -13496,18 +13481,18 @@
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B9" s="20"/>
-      <c r="C9" s="39" t="s">
-        <v>439</v>
+      <c r="C9" s="37" t="s">
+        <v>440</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="40" t="s">
-        <v>440</v>
+      <c r="F9" s="38" t="s">
+        <v>441</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
@@ -13515,16 +13500,16 @@
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
-      <c r="K9" s="35" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="10" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31" t="s">
+      <c r="K9" s="33" t="s">
         <v>442</v>
       </c>
-      <c r="C10" s="31"/>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="C10" s="30"/>
       <c r="D10" s="22"/>
       <c r="E10" s="20"/>
       <c r="F10" s="7"/>
@@ -13536,16 +13521,16 @@
     </row>
     <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B11" s="20"/>
-      <c r="C11" s="40" t="s">
-        <v>444</v>
+      <c r="C11" s="38" t="s">
+        <v>445</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="33" t="s">
-        <v>445</v>
+      <c r="F11" s="31" t="s">
+        <v>446</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
@@ -13555,18 +13540,18 @@
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B12" s="20"/>
-      <c r="C12" s="32" t="s">
-        <v>447</v>
+      <c r="C12" s="24" t="s">
+        <v>448</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="33" t="s">
-        <v>448</v>
+      <c r="F12" s="31" t="s">
+        <v>449</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20" t="s">
@@ -13576,12 +13561,12 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="C13" s="31"/>
+    <row r="13" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30" t="s">
+        <v>450</v>
+      </c>
+      <c r="C13" s="30"/>
       <c r="D13" s="22"/>
       <c r="E13" s="20"/>
       <c r="F13" s="7"/>
@@ -13591,18 +13576,18 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="32" t="s">
-        <v>451</v>
+      <c r="C14" s="24" t="s">
+        <v>452</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="33" t="s">
-        <v>452</v>
+      <c r="F14" s="31" t="s">
+        <v>453</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20" t="s">
@@ -13612,18 +13597,18 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B15" s="20"/>
-      <c r="C15" s="32" t="s">
-        <v>454</v>
+      <c r="C15" s="24" t="s">
+        <v>455</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="33" t="s">
-        <v>455</v>
+      <c r="F15" s="31" t="s">
+        <v>456</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20" t="s">
@@ -13635,16 +13620,16 @@
     </row>
     <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B16" s="20"/>
-      <c r="C16" s="39" t="s">
-        <v>457</v>
+      <c r="C16" s="37" t="s">
+        <v>458</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="20"/>
-      <c r="F16" s="40" t="s">
-        <v>458</v>
+      <c r="F16" s="38" t="s">
+        <v>459</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20" t="s">
@@ -13652,8 +13637,8 @@
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="35" t="s">
-        <v>441</v>
+      <c r="K16" s="33" t="s">
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -13671,15 +13656,15 @@
     <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D16" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D16" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3 E5:E16" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3 E5:E16" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5:H9 H11:H12 H14:H16" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3 H5:H9 H11:H12 H14:H16" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13703,9 +13688,9 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13722,10 +13707,10 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
@@ -13756,12 +13741,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31" t="s">
-        <v>459</v>
-      </c>
-      <c r="C2" s="31"/>
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2" s="30"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="7"/>
@@ -13771,18 +13756,18 @@
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="40" t="s">
-        <v>461</v>
+      <c r="C3" s="38" t="s">
+        <v>462</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="41" t="s">
-        <v>462</v>
+      <c r="F3" s="39" t="s">
+        <v>463</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -13792,18 +13777,18 @@
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B4" s="20"/>
-      <c r="C4" s="32" t="s">
-        <v>464</v>
+      <c r="C4" s="24" t="s">
+        <v>465</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
-      <c r="F4" s="33" t="s">
-        <v>465</v>
+      <c r="F4" s="31" t="s">
+        <v>466</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
@@ -13813,18 +13798,18 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="32" t="s">
-        <v>467</v>
+      <c r="C5" s="24" t="s">
+        <v>468</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
-      <c r="F5" s="33" t="s">
-        <v>468</v>
+      <c r="F5" s="31" t="s">
+        <v>469</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
@@ -13834,18 +13819,18 @@
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="32" t="s">
-        <v>470</v>
+      <c r="C6" s="24" t="s">
+        <v>471</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="33" t="s">
-        <v>471</v>
+      <c r="F6" s="31" t="s">
+        <v>472</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">
@@ -13855,12 +13840,12 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31" t="s">
-        <v>472</v>
-      </c>
-      <c r="C7" s="31"/>
+    <row r="7" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30" t="s">
+        <v>473</v>
+      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
       <c r="F7" s="7"/>
@@ -13870,18 +13855,18 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B8" s="20"/>
-      <c r="C8" s="32" t="s">
-        <v>474</v>
+      <c r="C8" s="24" t="s">
+        <v>475</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="33" t="s">
-        <v>475</v>
+      <c r="F8" s="31" t="s">
+        <v>476</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -13891,13 +13876,13 @@
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B9" s="20"/>
-      <c r="C9" s="32" t="s">
-        <v>477</v>
+      <c r="C9" s="24" t="s">
+        <v>478</v>
       </c>
       <c r="D9" s="9" t="n">
         <v>1</v>
@@ -13905,8 +13890,8 @@
       <c r="E9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>478</v>
+      <c r="F9" s="31" t="s">
+        <v>479</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
@@ -13916,39 +13901,39 @@
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B10" s="20"/>
-      <c r="C10" s="32" t="s">
-        <v>480</v>
+      <c r="C10" s="24" t="s">
+        <v>481</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
-      <c r="F10" s="33" t="s">
-        <v>481</v>
+      <c r="F10" s="31" t="s">
+        <v>482</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B11" s="20"/>
-      <c r="C11" s="32" t="s">
-        <v>483</v>
+      <c r="C11" s="24" t="s">
+        <v>484</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="33" t="s">
-        <v>484</v>
+      <c r="F11" s="31" t="s">
+        <v>485</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
@@ -13960,16 +13945,16 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B12" s="20"/>
-      <c r="C12" s="32" t="s">
-        <v>486</v>
+      <c r="C12" s="24" t="s">
+        <v>487</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="33" t="s">
-        <v>487</v>
+      <c r="F12" s="31" t="s">
+        <v>488</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20" t="s">
@@ -13979,12 +13964,12 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31" t="s">
-        <v>488</v>
-      </c>
-      <c r="C13" s="31"/>
+    <row r="13" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30" t="s">
+        <v>489</v>
+      </c>
+      <c r="C13" s="30"/>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
       <c r="F13" s="7"/>
@@ -13994,18 +13979,18 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="32" t="s">
-        <v>490</v>
+      <c r="C14" s="24" t="s">
+        <v>491</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="33" t="s">
-        <v>491</v>
+      <c r="F14" s="31" t="s">
+        <v>492</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20" t="s">
@@ -14015,18 +14000,18 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B15" s="20"/>
-      <c r="C15" s="32" t="s">
-        <v>493</v>
+      <c r="C15" s="24" t="s">
+        <v>494</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="33" t="s">
-        <v>494</v>
+      <c r="F15" s="31" t="s">
+        <v>495</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20" t="s">
@@ -14036,18 +14021,18 @@
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B16" s="20"/>
-      <c r="C16" s="32" t="s">
-        <v>496</v>
+      <c r="C16" s="24" t="s">
+        <v>497</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="33" t="s">
-        <v>497</v>
+      <c r="F16" s="31" t="s">
+        <v>498</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20" t="s">
@@ -14057,18 +14042,18 @@
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B17" s="20"/>
-      <c r="C17" s="32" t="s">
-        <v>499</v>
+      <c r="C17" s="24" t="s">
+        <v>500</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="33" t="s">
-        <v>500</v>
+      <c r="F17" s="31" t="s">
+        <v>501</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20" t="s">
@@ -14078,18 +14063,18 @@
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B18" s="20"/>
-      <c r="C18" s="32" t="s">
-        <v>502</v>
+      <c r="C18" s="24" t="s">
+        <v>503</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="33" t="s">
-        <v>503</v>
+      <c r="F18" s="31" t="s">
+        <v>504</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20" t="s">
@@ -14099,18 +14084,18 @@
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B19" s="20"/>
-      <c r="C19" s="32" t="s">
-        <v>505</v>
+      <c r="C19" s="24" t="s">
+        <v>506</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="33" t="s">
-        <v>506</v>
+      <c r="F19" s="31" t="s">
+        <v>507</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20" t="s">
@@ -14120,12 +14105,12 @@
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31" t="s">
-        <v>507</v>
-      </c>
-      <c r="C20" s="31"/>
+    <row r="20" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="29"/>
+      <c r="B20" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="C20" s="30"/>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
       <c r="F20" s="7"/>
@@ -14135,18 +14120,18 @@
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
     </row>
-    <row r="21" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B21" s="20"/>
-      <c r="C21" s="32" t="s">
-        <v>509</v>
+      <c r="C21" s="24" t="s">
+        <v>510</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="33" t="s">
-        <v>510</v>
+      <c r="F21" s="31" t="s">
+        <v>511</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20" t="s">
@@ -14156,18 +14141,18 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B22" s="20"/>
-      <c r="C22" s="32" t="s">
-        <v>512</v>
+      <c r="C22" s="24" t="s">
+        <v>513</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="33" t="s">
-        <v>513</v>
+      <c r="F22" s="31" t="s">
+        <v>514</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20" t="s">
@@ -14177,12 +14162,12 @@
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" s="4" customFormat="true" ht="16.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="30"/>
-      <c r="B23" s="31" t="s">
-        <v>514</v>
-      </c>
-      <c r="C23" s="31"/>
+    <row r="23" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="29"/>
+      <c r="B23" s="30" t="s">
+        <v>515</v>
+      </c>
+      <c r="C23" s="30"/>
       <c r="D23" s="22"/>
       <c r="E23" s="23"/>
       <c r="F23" s="7"/>
@@ -14192,18 +14177,18 @@
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
     </row>
-    <row r="24" customFormat="false" ht="93.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="93.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B24" s="20"/>
-      <c r="C24" s="40" t="s">
-        <v>516</v>
+      <c r="C24" s="38" t="s">
+        <v>517</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="23"/>
-      <c r="F24" s="33" t="s">
-        <v>517</v>
+      <c r="F24" s="31" t="s">
+        <v>518</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20" t="s">
@@ -14213,13 +14198,13 @@
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" customFormat="false" ht="57" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B25" s="20"/>
-      <c r="C25" s="32" t="s">
-        <v>519</v>
+      <c r="C25" s="24" t="s">
+        <v>520</v>
       </c>
       <c r="D25" s="22" t="n">
         <v>1</v>
@@ -14227,8 +14212,8 @@
       <c r="E25" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="33" t="s">
-        <v>520</v>
+      <c r="F25" s="31" t="s">
+        <v>521</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20" t="s">
@@ -14238,18 +14223,18 @@
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B26" s="20"/>
-      <c r="C26" s="32" t="s">
-        <v>522</v>
+      <c r="C26" s="24" t="s">
+        <v>523</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="23"/>
-      <c r="F26" s="33" t="s">
-        <v>523</v>
+      <c r="F26" s="31" t="s">
+        <v>524</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20" t="s">
@@ -14261,16 +14246,16 @@
     </row>
     <row r="27" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B27" s="20"/>
-      <c r="C27" s="32" t="s">
-        <v>525</v>
+      <c r="C27" s="24" t="s">
+        <v>526</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="23"/>
-      <c r="F27" s="33" t="s">
-        <v>526</v>
+      <c r="F27" s="31" t="s">
+        <v>527</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20" t="s">
@@ -14280,18 +14265,18 @@
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B28" s="20"/>
-      <c r="C28" s="32" t="s">
-        <v>528</v>
+      <c r="C28" s="24" t="s">
+        <v>529</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="33" t="s">
-        <v>529</v>
+      <c r="F28" s="31" t="s">
+        <v>530</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20" t="s">
@@ -14301,18 +14286,18 @@
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B29" s="20"/>
-      <c r="C29" s="32" t="s">
-        <v>531</v>
+      <c r="C29" s="24" t="s">
+        <v>532</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="33" t="s">
-        <v>532</v>
+      <c r="F29" s="31" t="s">
+        <v>533</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20" t="s">
@@ -14322,39 +14307,39 @@
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B30" s="20"/>
-      <c r="C30" s="32" t="s">
-        <v>534</v>
+      <c r="C30" s="24" t="s">
+        <v>535</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="33" t="s">
-        <v>535</v>
+      <c r="F30" s="31" t="s">
+        <v>536</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
       <c r="K30" s="20" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="28.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B31" s="20"/>
-      <c r="C31" s="32" t="s">
-        <v>537</v>
+      <c r="C31" s="24" t="s">
+        <v>538</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="33" t="s">
-        <v>538</v>
+      <c r="F31" s="31" t="s">
+        <v>539</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20" t="s">
@@ -14364,18 +14349,18 @@
       <c r="J31" s="20"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B32" s="20"/>
-      <c r="C32" s="32" t="s">
-        <v>540</v>
+      <c r="C32" s="24" t="s">
+        <v>541</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="33" t="s">
-        <v>541</v>
+      <c r="F32" s="31" t="s">
+        <v>542</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20" t="s">
@@ -14385,13 +14370,13 @@
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B33" s="20"/>
-      <c r="C33" s="32" t="s">
-        <v>543</v>
+      <c r="C33" s="24" t="s">
+        <v>544</v>
       </c>
       <c r="D33" s="9" t="n">
         <v>1</v>
@@ -14399,8 +14384,8 @@
       <c r="E33" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="33" t="s">
-        <v>544</v>
+      <c r="F33" s="31" t="s">
+        <v>545</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20" t="s">
@@ -14412,16 +14397,16 @@
     </row>
     <row r="34" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B34" s="20"/>
-      <c r="C34" s="32" t="s">
-        <v>546</v>
+      <c r="C34" s="24" t="s">
+        <v>547</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="23"/>
-      <c r="F34" s="33" t="s">
-        <v>547</v>
+      <c r="F34" s="31" t="s">
+        <v>548</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20" t="s">
@@ -14433,16 +14418,16 @@
     </row>
     <row r="35" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B35" s="20"/>
-      <c r="C35" s="32" t="s">
-        <v>549</v>
+      <c r="C35" s="24" t="s">
+        <v>550</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="23"/>
-      <c r="F35" s="33" t="s">
-        <v>550</v>
+      <c r="F35" s="31" t="s">
+        <v>551</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="20" t="s">
@@ -14452,18 +14437,18 @@
       <c r="J35" s="20"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B36" s="20"/>
-      <c r="C36" s="40" t="s">
-        <v>552</v>
+      <c r="C36" s="38" t="s">
+        <v>553</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="33" t="s">
-        <v>553</v>
+      <c r="F36" s="31" t="s">
+        <v>554</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20" t="s">
@@ -14473,18 +14458,18 @@
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B37" s="20"/>
-      <c r="C37" s="32" t="s">
-        <v>555</v>
+      <c r="C37" s="24" t="s">
+        <v>556</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="23"/>
-      <c r="F37" s="33" t="s">
-        <v>556</v>
+      <c r="F37" s="31" t="s">
+        <v>557</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20" t="s">
@@ -14496,16 +14481,16 @@
     </row>
     <row r="38" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B38" s="20"/>
-      <c r="C38" s="32" t="s">
-        <v>558</v>
+      <c r="C38" s="24" t="s">
+        <v>559</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="23"/>
-      <c r="F38" s="33" t="s">
-        <v>559</v>
+      <c r="F38" s="31" t="s">
+        <v>560</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20" t="s">
@@ -14515,13 +14500,13 @@
       <c r="J38" s="20"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="20" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B39" s="20"/>
-      <c r="C39" s="32" t="s">
-        <v>561</v>
+      <c r="C39" s="24" t="s">
+        <v>562</v>
       </c>
       <c r="D39" s="9" t="n">
         <v>2</v>
@@ -14529,8 +14514,8 @@
       <c r="E39" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F39" s="33" t="s">
-        <v>562</v>
+      <c r="F39" s="31" t="s">
+        <v>563</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20" t="s">
@@ -14542,16 +14527,16 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B40" s="20"/>
-      <c r="C40" s="32" t="s">
-        <v>564</v>
+      <c r="C40" s="24" t="s">
+        <v>565</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="23"/>
-      <c r="F40" s="33" t="s">
-        <v>565</v>
+      <c r="F40" s="31" t="s">
+        <v>566</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="20" t="s">
@@ -14563,11 +14548,11 @@
     </row>
     <row r="41" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="20" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B41" s="20"/>
-      <c r="C41" s="32" t="s">
-        <v>567</v>
+      <c r="C41" s="24" t="s">
+        <v>568</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="23"/>
@@ -14600,15 +14585,15 @@
     <mergeCell ref="B23:C23"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D41" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D41" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:H6 H8:H12 H14:H19 H21:H22 H24:H41" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:H6 H8:H12 H14:H19 H21:H22 H24:H41" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E6 E8:E41" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E6 E8:E41" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -14637,23 +14622,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="66.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="42" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="66.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
@@ -14663,7 +14650,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="22"/>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="22" t="s">
@@ -14684,15 +14671,15 @@
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B2" s="20"/>
-      <c r="C2" s="40" t="s">
-        <v>569</v>
+      <c r="C2" s="38" t="s">
+        <v>570</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="44"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -14701,11 +14688,11 @@
     </row>
     <row r="3" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="32" t="s">
-        <v>571</v>
+      <c r="C3" s="24" t="s">
+        <v>572</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
@@ -14718,11 +14705,11 @@
     </row>
     <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B4" s="20"/>
-      <c r="C4" s="32" t="s">
-        <v>573</v>
+      <c r="C4" s="24" t="s">
+        <v>574</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
@@ -14735,11 +14722,11 @@
     </row>
     <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="32" t="s">
-        <v>575</v>
+      <c r="C5" s="24" t="s">
+        <v>576</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
@@ -14752,11 +14739,11 @@
     </row>
     <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="32" t="s">
-        <v>577</v>
+      <c r="C6" s="24" t="s">
+        <v>578</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
@@ -14769,11 +14756,11 @@
     </row>
     <row r="7" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="32" t="s">
-        <v>579</v>
+      <c r="C7" s="24" t="s">
+        <v>580</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="23"/>
@@ -14811,15 +14798,15 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D7" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H7" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E7" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -14847,148 +14834,148 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="71.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="45" width="25.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="6.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="45" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="45" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="71.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="25.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="6.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="40" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1" s="46" t="s">
-        <v>580</v>
-      </c>
-      <c r="D1" s="47" t="s">
+      <c r="C1" s="41" t="s">
         <v>581</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="D1" s="42" t="s">
+        <v>582</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="48" t="s">
-        <v>582</v>
-      </c>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="43" t="s">
         <v>583</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="44" t="s">
         <v>584</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="D2" s="45" t="s">
+        <v>585</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="51" t="s">
-        <v>585</v>
-      </c>
-      <c r="C3" s="52" t="s">
+      <c r="B3" s="46" t="s">
         <v>586</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="C3" s="47" t="s">
         <v>587</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="D3" s="48" t="s">
         <v>588</v>
       </c>
+      <c r="E3" s="49" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="55" t="s">
-        <v>589</v>
-      </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57" t="n">
+      <c r="B4" s="50" t="s">
+        <v>590</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="58" t="s">
-        <v>590</v>
-      </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57" t="n">
+      <c r="B5" s="53" t="s">
+        <v>591</v>
+      </c>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="56"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="59" t="s">
-        <v>591</v>
-      </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="57" t="n">
+      <c r="B6" s="54" t="s">
+        <v>592</v>
+      </c>
+      <c r="C6" s="51"/>
+      <c r="D6" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="56"/>
+      <c r="E6" s="51"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="58" t="s">
-        <v>592</v>
-      </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="57" t="n">
+      <c r="B7" s="53" t="s">
+        <v>593</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="56"/>
+      <c r="E7" s="51"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="58" t="s">
-        <v>593</v>
-      </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="57" t="n">
+      <c r="B8" s="53" t="s">
+        <v>594</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="56"/>
+      <c r="E8" s="51"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="58" t="s">
-        <v>594</v>
-      </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="57" t="n">
+      <c r="B9" s="53" t="s">
+        <v>595</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="56"/>
+      <c r="E9" s="51"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="58" t="s">
-        <v>595</v>
-      </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="57" t="n">
+      <c r="B10" s="53" t="s">
+        <v>596</v>
+      </c>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="56"/>
+      <c r="E10" s="51"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="60" t="s">
-        <v>596</v>
-      </c>
-      <c r="D11" s="61" t="n">
+      <c r="C11" s="55" t="s">
+        <v>597</v>
+      </c>
+      <c r="D11" s="56" t="n">
         <f aca="false">SUM(D4:D10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="45" t="s">
-        <v>597</v>
-      </c>
-      <c r="D12" s="62" t="n">
+      <c r="C12" s="40" t="s">
+        <v>598</v>
+      </c>
+      <c r="D12" s="57" t="n">
         <f aca="false">COUNT(D4:D10)</f>
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="45" t="s">
-        <v>598</v>
-      </c>
-      <c r="D13" s="63" t="n">
+      <c r="C13" s="40" t="s">
+        <v>599</v>
+      </c>
+      <c r="D13" s="58" t="n">
         <f aca="false">IFERROR(D11/(D12*2), 0)</f>
         <v>0</v>
       </c>
@@ -14999,7 +14986,7 @@
     <mergeCell ref="D2:H2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D10" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D10" type="list">
       <formula1>"0,1,2"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -15022,7 +15009,7 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -15040,10 +15027,10 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
@@ -15075,11 +15062,11 @@
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31" t="s">
-        <v>599</v>
-      </c>
-      <c r="C2" s="31"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>600</v>
+      </c>
+      <c r="C2" s="30"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="7"/>
@@ -15091,16 +15078,16 @@
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="32" t="s">
-        <v>601</v>
+      <c r="C3" s="24" t="s">
+        <v>602</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
-      <c r="F3" s="32" t="s">
-        <v>602</v>
+      <c r="F3" s="24" t="s">
+        <v>603</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -15112,16 +15099,16 @@
     </row>
     <row r="4" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B4" s="20"/>
-      <c r="C4" s="64" t="s">
-        <v>604</v>
+      <c r="C4" s="59" t="s">
+        <v>605</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
-      <c r="F4" s="32" t="s">
-        <v>605</v>
+      <c r="F4" s="24" t="s">
+        <v>606</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
@@ -15133,16 +15120,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="32" t="s">
-        <v>607</v>
+      <c r="C5" s="24" t="s">
+        <v>608</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
-      <c r="F5" s="32" t="s">
-        <v>608</v>
+      <c r="F5" s="24" t="s">
+        <v>609</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
@@ -15154,16 +15141,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="32" t="s">
-        <v>610</v>
+      <c r="C6" s="24" t="s">
+        <v>611</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="32" t="s">
-        <v>611</v>
+      <c r="F6" s="24" t="s">
+        <v>612</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">
@@ -15179,16 +15166,16 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H6" type="list">
-      <formula1>Selections!$C$4:$C$9</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D6" type="list">
+      <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E6" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D6" type="list">
-      <formula1>Selections!$A$4:$A$7</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H6" type="list">
+      <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Label column E as "Rank" in the SQ sheet
The new "Software Quality" (SQ) sheet should have the same column
names as it does in every other sheet: "Rank".  However, when I
created the new sheet (see commit 9ba5431bf and commit 77c8619a8a),
I forgot to give that column a title.  This commit fixes that.
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FUNC Reqs" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="614">
   <si>
     <t xml:space="preserve">Requirement ID Number</t>
   </si>
@@ -2968,9 +2968,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1913040</xdr:colOff>
+      <xdr:colOff>1912680</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2980,7 +2980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635400" y="0"/>
-          <a:ext cx="1912320" cy="675360"/>
+          <a:ext cx="1911960" cy="675000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3036,7 +3036,7 @@
   <dimension ref="A1:AMJ111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
     </sheetView>
@@ -12732,7 +12732,7 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -13688,7 +13688,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -14616,8 +14616,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14649,7 +14649,9 @@
       <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22"/>
+      <c r="E1" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
@@ -15009,7 +15011,7 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add a category row to the "SQ" sheet
The new row just says "1.  Software Quality and Maintainability",
which just repeats what the "SQ" sheet is about, but the presence of
this row before any of the actual requirements causes this sheet to
match the pattern of the other sheets, in which a category description
always comes before the requirements in that category.
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="615">
   <si>
     <t xml:space="preserve">Requirement ID Number</t>
   </si>
@@ -2193,6 +2193,9 @@
   </si>
   <si>
     <t xml:space="preserve">The PSM shall be secure from unauthorized access or use, and shall sanitize inputs and outputs where possible so as to avoid compromising itself or other systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  Software Quality and Maintainability</t>
   </si>
   <si>
     <t xml:space="preserve">psm-SQ-1.1</t>
@@ -2968,9 +2971,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1912680</xdr:colOff>
+      <xdr:colOff>1912320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2980,7 +2983,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635400" y="0"/>
-          <a:ext cx="1911960" cy="675000"/>
+          <a:ext cx="1911600" cy="674640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11828,7 +11831,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
@@ -14617,7 +14620,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14671,47 +14674,45 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+    <row r="2" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29" t="s">
         <v>569</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+    </row>
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
         <v>570</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="38" t="s">
         <v>571</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="24" t="s">
-        <v>572</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="24" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
@@ -14722,13 +14723,13 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="24" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
@@ -14739,13 +14740,13 @@
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="24" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
@@ -14756,15 +14757,15 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="24" t="s">
-        <v>580</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>579</v>
+      </c>
+      <c r="D7" s="22"/>
       <c r="E7" s="23"/>
       <c r="F7" s="24"/>
       <c r="G7" s="20"/>
@@ -14773,7 +14774,23 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="24" t="s">
+        <v>581</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+    </row>
     <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -14800,15 +14817,15 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D8" type="list">
       <formula1>Selections!$A$4:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:H8" type="list">
       <formula1>Selections!$C$4:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E8" type="list">
       <formula1>Selections!$B$4:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -14846,10 +14863,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C1" s="41" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
@@ -14858,13 +14875,13 @@
     </row>
     <row r="2" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="43" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
@@ -14873,21 +14890,21 @@
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="46" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="50" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="52" t="n">
@@ -14897,7 +14914,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="53" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="52" t="n">
@@ -14907,7 +14924,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="54" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="52" t="n">
@@ -14917,7 +14934,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="53" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C7" s="51"/>
       <c r="D7" s="52" t="n">
@@ -14927,7 +14944,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="53" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C8" s="51"/>
       <c r="D8" s="52" t="n">
@@ -14937,7 +14954,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="53" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C9" s="51"/>
       <c r="D9" s="52" t="n">
@@ -14947,7 +14964,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="53" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C10" s="51"/>
       <c r="D10" s="52" t="n">
@@ -14957,7 +14974,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="55" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D11" s="56" t="n">
         <f aca="false">SUM(D4:D10)</f>
@@ -14966,7 +14983,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="40" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D12" s="57" t="n">
         <f aca="false">COUNT(D4:D10)</f>
@@ -14975,7 +14992,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="40" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D13" s="58" t="n">
         <f aca="false">IFERROR(D11/(D12*2), 0)</f>
@@ -15066,7 +15083,7 @@
     <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29"/>
       <c r="B2" s="30" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="22"/>
@@ -15080,16 +15097,16 @@
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="24" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="24" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -15101,16 +15118,16 @@
     </row>
     <row r="4" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="59" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="24" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
@@ -15122,16 +15139,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="24" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
       <c r="F5" s="24" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
@@ -15143,16 +15160,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="24" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
       <c r="F6" s="24" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">

</xml_diff>

<commit_message>
Remove spurious row from IA sheet
Row 23 in the IA sheet had "How do PSM interface to NPI?" in the
"Source Document" column (column G) but no other fields.  At the very
least this question was in the wrong column, but it also didn't add
anything useful to our understanding of the PSM's requirements, so I
just removed it.
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FUNC Reqs" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Access and Delivery'!$H$1:$H$40</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'FUNC Reqs'!$H$1:$H$110</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Information Architecture'!$H$1:$H$23</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Information Architecture'!$H$1:$H$22</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Integration and Utility'!$H$1:$H$16</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Intermediary &amp; Interface'!$H$1:$H$17</definedName>
     <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'Pharmacy (MMIS)'!$H$1:$H$6</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="614">
   <si>
     <t xml:space="preserve">Requirement ID Number</t>
   </si>
@@ -1736,9 +1736,6 @@
   </si>
   <si>
     <t xml:space="preserve">TA.SP.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How do PSM interface to NPI?</t>
   </si>
   <si>
     <t xml:space="preserve">1.  Technical Service Classification:  Configuration Management</t>
@@ -11831,7 +11828,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
@@ -12733,10 +12730,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13230,13 +13227,9 @@
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="0" t="s">
-        <v>420</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="H1:H23">
+  <autoFilter ref="H1:H22">
     <filterColumn colId="0">
       <customFilters and="true">
         <customFilter operator="equal" val="MVP - Dec"/>
@@ -13338,7 +13331,7 @@
     <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29"/>
       <c r="B2" s="30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="22"/>
@@ -13352,11 +13345,11 @@
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>1</v>
@@ -13365,7 +13358,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -13378,7 +13371,7 @@
     <row r="4" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29"/>
       <c r="B4" s="30" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="22"/>
@@ -13392,16 +13385,16 @@
     </row>
     <row r="5" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="20"/>
       <c r="F5" s="31" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
@@ -13410,16 +13403,16 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="33" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="24" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>2</v>
@@ -13428,7 +13421,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">
@@ -13440,16 +13433,16 @@
     </row>
     <row r="7" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="24" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="20"/>
       <c r="F7" s="31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20" t="s">
@@ -13461,11 +13454,11 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="24" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D8" s="9" t="n">
         <v>3</v>
@@ -13474,7 +13467,7 @@
         <v>52</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -13486,16 +13479,16 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="37" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="20"/>
       <c r="F9" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
@@ -13504,13 +13497,13 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="33" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="29"/>
       <c r="B10" s="30" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="22"/>
@@ -13524,16 +13517,16 @@
     </row>
     <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="20"/>
       <c r="F11" s="31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
@@ -13545,16 +13538,16 @@
     </row>
     <row r="12" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="24" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="20"/>
       <c r="F12" s="31" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20" t="s">
@@ -13567,7 +13560,7 @@
     <row r="13" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="22"/>
@@ -13581,16 +13574,16 @@
     </row>
     <row r="14" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="20"/>
       <c r="F14" s="31" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20" t="s">
@@ -13602,16 +13595,16 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="20"/>
       <c r="F15" s="31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20" t="s">
@@ -13623,16 +13616,16 @@
     </row>
     <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="37" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="20"/>
       <c r="F16" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20" t="s">
@@ -13641,7 +13634,7 @@
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="33" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -13747,7 +13740,7 @@
     <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29"/>
       <c r="B2" s="30" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="22"/>
@@ -13761,16 +13754,16 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
       <c r="F3" s="39" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -13782,16 +13775,16 @@
     </row>
     <row r="4" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="24" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
       <c r="F4" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
@@ -13803,16 +13796,16 @@
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="24" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
       <c r="F5" s="31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
@@ -13824,16 +13817,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="24" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
       <c r="F6" s="31" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">
@@ -13846,7 +13839,7 @@
     <row r="7" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="29"/>
       <c r="B7" s="30" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="22"/>
@@ -13860,16 +13853,16 @@
     </row>
     <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="24" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="23"/>
       <c r="F8" s="31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -13881,11 +13874,11 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="24" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D9" s="9" t="n">
         <v>1</v>
@@ -13894,7 +13887,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20" t="s">
@@ -13906,16 +13899,16 @@
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="24" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
       <c r="F10" s="31" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
@@ -13927,16 +13920,16 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="24" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="23"/>
       <c r="F11" s="31" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
@@ -13948,16 +13941,16 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="24" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="23"/>
       <c r="F12" s="31" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20" t="s">
@@ -13970,7 +13963,7 @@
     <row r="13" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="22"/>
@@ -13984,16 +13977,16 @@
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="24" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
       <c r="F14" s="31" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20" t="s">
@@ -14005,16 +13998,16 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="24" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
       <c r="F15" s="31" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20" t="s">
@@ -14026,16 +14019,16 @@
     </row>
     <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="24" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
       <c r="F16" s="31" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20" t="s">
@@ -14047,16 +14040,16 @@
     </row>
     <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="24" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
       <c r="F17" s="31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20" t="s">
@@ -14068,16 +14061,16 @@
     </row>
     <row r="18" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="24" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
       <c r="F18" s="31" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20" t="s">
@@ -14089,16 +14082,16 @@
     </row>
     <row r="19" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="24" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
       <c r="F19" s="31" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20" t="s">
@@ -14111,7 +14104,7 @@
     <row r="20" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="29"/>
       <c r="B20" s="30" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="22"/>
@@ -14125,16 +14118,16 @@
     </row>
     <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="23"/>
       <c r="F21" s="31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20" t="s">
@@ -14146,16 +14139,16 @@
     </row>
     <row r="22" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
       <c r="F22" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20" t="s">
@@ -14168,7 +14161,7 @@
     <row r="23" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="29"/>
       <c r="B23" s="30" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="22"/>
@@ -14182,16 +14175,16 @@
     </row>
     <row r="24" customFormat="false" ht="93.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="38" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="23"/>
       <c r="F24" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20" t="s">
@@ -14203,11 +14196,11 @@
     </row>
     <row r="25" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="24" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D25" s="22" t="n">
         <v>1</v>
@@ -14216,7 +14209,7 @@
         <v>29</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20" t="s">
@@ -14228,16 +14221,16 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="24" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="23"/>
       <c r="F26" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20" t="s">
@@ -14249,16 +14242,16 @@
     </row>
     <row r="27" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="24" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="23"/>
       <c r="F27" s="31" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20" t="s">
@@ -14270,16 +14263,16 @@
     </row>
     <row r="28" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="24" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="23"/>
       <c r="F28" s="31" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20" t="s">
@@ -14291,16 +14284,16 @@
     </row>
     <row r="29" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="24" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="23"/>
       <c r="F29" s="31" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20" t="s">
@@ -14312,16 +14305,16 @@
     </row>
     <row r="30" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="24" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23"/>
       <c r="F30" s="31" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
@@ -14333,16 +14326,16 @@
     </row>
     <row r="31" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="24" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="23"/>
       <c r="F31" s="31" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20" t="s">
@@ -14354,16 +14347,16 @@
     </row>
     <row r="32" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="24" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="23"/>
       <c r="F32" s="31" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20" t="s">
@@ -14375,11 +14368,11 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="24" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D33" s="9" t="n">
         <v>1</v>
@@ -14388,7 +14381,7 @@
         <v>20</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20" t="s">
@@ -14400,16 +14393,16 @@
     </row>
     <row r="34" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="24" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="23"/>
       <c r="F34" s="31" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20" t="s">
@@ -14421,16 +14414,16 @@
     </row>
     <row r="35" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="24" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="23"/>
       <c r="F35" s="31" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="20" t="s">
@@ -14442,16 +14435,16 @@
     </row>
     <row r="36" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="38" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="23"/>
       <c r="F36" s="31" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20" t="s">
@@ -14463,16 +14456,16 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="24" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="23"/>
       <c r="F37" s="31" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20" t="s">
@@ -14484,16 +14477,16 @@
     </row>
     <row r="38" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="24" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="23"/>
       <c r="F38" s="31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20" t="s">
@@ -14505,11 +14498,11 @@
     </row>
     <row r="39" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="24" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D39" s="9" t="n">
         <v>2</v>
@@ -14518,7 +14511,7 @@
         <v>52</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20" t="s">
@@ -14530,16 +14523,16 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="24" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="23"/>
       <c r="F40" s="31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="20" t="s">
@@ -14551,11 +14544,11 @@
     </row>
     <row r="41" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="20" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="24" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="23"/>
@@ -14619,7 +14612,7 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -14677,7 +14670,7 @@
     <row r="2" s="4" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29"/>
       <c r="B2" s="29" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -14691,11 +14684,11 @@
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="38" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
@@ -14708,11 +14701,11 @@
     </row>
     <row r="4" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="24" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
@@ -14725,11 +14718,11 @@
     </row>
     <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="24" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
@@ -14742,11 +14735,11 @@
     </row>
     <row r="6" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="24" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
@@ -14759,11 +14752,11 @@
     </row>
     <row r="7" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="24" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
@@ -14776,11 +14769,11 @@
     </row>
     <row r="8" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="24" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="23"/>
@@ -14863,10 +14856,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C1" s="41" t="s">
+        <v>581</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>582</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>583</v>
       </c>
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
@@ -14875,13 +14868,13 @@
     </row>
     <row r="2" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="43" t="s">
+        <v>583</v>
+      </c>
+      <c r="C2" s="44" t="s">
         <v>584</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>585</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>586</v>
       </c>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
@@ -14890,21 +14883,21 @@
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="46" t="s">
+        <v>586</v>
+      </c>
+      <c r="C3" s="47" t="s">
         <v>587</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="D3" s="48" t="s">
         <v>588</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="E3" s="49" t="s">
         <v>589</v>
-      </c>
-      <c r="E3" s="49" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="50" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="52" t="n">
@@ -14914,7 +14907,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="53" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="52" t="n">
@@ -14924,7 +14917,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="54" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="52" t="n">
@@ -14934,7 +14927,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="53" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C7" s="51"/>
       <c r="D7" s="52" t="n">
@@ -14944,7 +14937,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="53" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C8" s="51"/>
       <c r="D8" s="52" t="n">
@@ -14954,7 +14947,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="53" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C9" s="51"/>
       <c r="D9" s="52" t="n">
@@ -14964,7 +14957,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="53" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C10" s="51"/>
       <c r="D10" s="52" t="n">
@@ -14974,7 +14967,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="55" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D11" s="56" t="n">
         <f aca="false">SUM(D4:D10)</f>
@@ -14983,7 +14976,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="40" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D12" s="57" t="n">
         <f aca="false">COUNT(D4:D10)</f>
@@ -14992,7 +14985,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="40" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D13" s="58" t="n">
         <f aca="false">IFERROR(D11/(D12*2), 0)</f>
@@ -15083,7 +15076,7 @@
     <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29"/>
       <c r="B2" s="30" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="22"/>
@@ -15097,16 +15090,16 @@
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="24" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
@@ -15118,16 +15111,16 @@
     </row>
     <row r="4" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="59" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
@@ -15139,16 +15132,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="24" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
       <c r="F5" s="24" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20" t="s">
@@ -15160,16 +15153,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="24" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
       <c r="F6" s="24" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20" t="s">

</xml_diff>

<commit_message>
Update psm-SQ-1.3 to include formats as well as libraries.
This is to make that req applicable to things like issue #613.
</commit_message>
<xml_diff>
--- a/requirements/RTM.xlsx
+++ b/requirements/RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FUNC Reqs" sheetId="1" state="visible" r:id="rId2"/>
@@ -2210,7 +2210,7 @@
     <t xml:space="preserve">psm-SQ-1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">The PSM shall use modern source code dependency management techniques, and shall use up-to-date versions of upstream third-party dependencies.</t>
+    <t xml:space="preserve">The PSM shall use modern source code dependency management techniques, and shall use up-to-date versions of upstream third-party dependencies and formats.</t>
   </si>
   <si>
     <t xml:space="preserve">psm-SQ-1.4</t>
@@ -2968,9 +2968,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1912320</xdr:colOff>
+      <xdr:colOff>1911960</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2980,7 +2980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635400" y="0"/>
-          <a:ext cx="1911600" cy="674640"/>
+          <a:ext cx="1911240" cy="674280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12366,7 +12366,7 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -14612,8 +14612,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>